<commit_message>
Add code for running base model, training the model, and testing the model in LLM.ipynb
</commit_message>
<xml_diff>
--- a/DataInputs/LLM-Training-Dataset/example_training_data.xlsx
+++ b/DataInputs/LLM-Training-Dataset/example_training_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,66 +460,527 @@
         <is>
           <t xml:space="preserve">Week Ending on 2023-02-03:
 News Summary:
-1. Nick 'Nickmercs' Kolcheff Wants To Be Gaming's First Business Mogul - 2023-01-30: The 32-year-old gamer is on a never-ending quest for more wins, more deals and more money, even as viewership declines and exclusive streaming deals disappear., Author: Matt Craig, Source: Forbes, Sentiment Score: 0.116702
-2. Social commerce market 2023-2027: A descriptive analysis of five forces model, market dynamics, and segmentation- Technavio - 2023-01-30: NEW YORK, Jan. 30, 2023 /PRNewswire/ -- According to Technavio, the global social commerce market size is estimated to grow by from 2022 to 2027. The market is estimated to grow at a CAGR of almost 31% during the forecast period. APAC will account for the largest share of the global market during ..., Author: PRNewswire, Source: Benzinga, Sentiment Score: 0.184888
-3. 1 Bargain-Basement Warren Buffett Stock Down 59% to Buy Before It Starts Soaring - 2023-01-30: Cloud computing is just part of the attraction., Author: Danny Vena, Source: Motley Fool, Sentiment Score: 0.230527
-4. Big Tech's squeeze of technology innovators is costing you more for apps and other internet services - 2023-01-30: Change intellectual property law to help level the playing field or risk America's global tech leadership., Author: Mike Feibus, Source: MarketWatch, Sentiment Score: 0.188588
-5. Marathon Petroleum Corporation announces election of new director - 2023-01-30: FINDLAY, Ohio, Jan. 30, 2023 /PRNewswire/ -- Marathon Petroleum Corp. ( NYSE: MPC ) today announced that Toni Townes-Whitley has been elected to the company's board of directors, effective March 1, 2023. Townes-Whitley is a global technology leader whose career spans more than 35 years, most ..., Author: Marathon Petroleum Corporation, Source: PR Newswire, Sentiment Score: 0.298622
-6. Here's why you should always wait for the earnings call | Business - 2023-01-30: Here's why you should always wait for the earnings call ..., Author: Nicole Goodkind, Source: CNN, Sentiment Score: -0.100504
-7. Best Leveraged ETF Areas of Last Week - 2023-01-30: Wall Street was modestly upbeat last week. The S&amp;P 500, the Dow Jones, the Nasdaq and the Russell 2000 added 2.5%, 1.8%, 4.3% and 2.4% last week, respectively., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.115604
-8. Think Chevron's Profit Was Obscene? 5 Companies Will Blow It Away - 2023-01-30: Chevron's ( CVX ) giant $36.5 billion 2022 profit certainly turned heads - including at the White House. But plenty of S&amp;P 500 companies will make even more than the oil giant. The bulk of S&amp;P 500 companies this week will report their fourth-quarter and full 2022 results., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.31514
-9. Sensor Data Analytics Market Size is Projected to Reach USD 6.26 Billion at a CAGR of 24.42% by 2030 - Report by Market Research Future  ( MRFR )  - 2023-01-30: New York, US, Jan. 30, 2023 ( GLOBE NEWSWIRE ) -- According to a comprehensive research report by Market Research Future ( MRFR ) , The global sensor data analytics market - By Components, By Services, By Application - Is forecast for 2030., Author: Globe Newswire, Source: Benzinga, Sentiment Score: 0.261246
-10. Tech Futures Sell Off With Fed Meeting In Sight - 2023-01-30: Dow Jones Futures Fall With Fed Meeting In Sight. Tesla Stock ... Investor's Business Daily ..., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.200889
-11. Arrival Appoints Igor Torgov as CEO and Announces Significant Savings Initiatives to Reduce Spend by Approximately 50% - 2023-01-30: LUXEMBOURG, Jan. 30, 2023 ( GLOBE NEWSWIRE ) -- Arrival ( NASDAQ: ARVL ) today announces the appointment of Igor Torgov, former Arrival EVP of Digital, as CEO. The Board has unanimously voted in Igor to effect the planned restructuring of its business and to support Arrival's mission to master a ..., Author: Arrival Group, Source: GlobeNewswire, Sentiment Score: 0.321889
-12. Data Catalog Market Size Hits $1.8 Billion by 2027, growing at a CAGR of 22.0%: Report by MarketsandMarkets - 2023-01-30: Chicago, Jan. 30, 2023 ( GLOBE NEWSWIRE ) -- The global Data Catalog Market size is expected to grow from USD 0.7 billion in 2022 to USD 1.8 billion in 2027, at a Compound Annual Growth Rate ( CAGR ) of 22.0% during the forecast period, according to a new report by MarketsandMarkets™., Author: Globe Newswire, Source: Benzinga, Sentiment Score: 0.263356
-13. Bayen Group Receives Partner of the Year Award - 2023-01-30: LOS ANGELES, Jan. 30, 2023 /PRNewswire/ -- Bayen Group, LLC was awarded Partner of the Year by Burns &amp; McDonnell. They were presented this award at the Burns &amp; McDonnell annual Empowering Diverse Partnerships Awards event in Kansas City, Missouri on January 12, 2023., Author: Bayen Group, Source: PR Newswire, Sentiment Score: 0.164626
-14. Data center market to grow by 20.22% Y-O-Y from 2021 to 2022: Rise in adoption of multi-cloud and network upgrades to support 5G will drive growth - Technavio - 2023-01-30: Data center market to grow by 20.22% Y-O-Y from 2021 to 2022 ... PR ..., Author: Technavio, Source: PR Newswire, Sentiment Score: 0.271381
-15. Velixo Highlights Record-Breaking Results and Strong Momentum at Acumatica Summit 2023 - 2023-01-30: Velixo Highlights Record-Breaking Results and Strong Momentum ... PR ..., Author: Velixo, Source: PR Newswire, Sentiment Score: 0.416012
-16. Investors Heavily Search Microsoft Corporation  ( MSFT ) : Here is What You Need to Know - 2023-01-30: Recently, Zacks.com users have been paying close attention to Microsoft (MSFT). This makes it worthwhile to examine what the stock has in store., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.223909
-17. Big Tech Earnings Are Almost Here. Microsoft Has Investors on Edge. - 2023-01-30: Apple, Amazon, and Other Big Tech Earnings Are Coming. What to Expect. ..., Author: Eric J. Savitz, Source: Barrons, Sentiment Score: -0.093211
-18. DocuSign expands leadership team with newly created roles across strategy, marketing &amp; growth - 2023-01-30: DocuSign expands leadership team with newly created roles across ... PR ..., Author: DocuSign, Source: PR Newswire, Sentiment Score: 0.372439
-19. Tech Stocks, On Best Run Since 2001, Face Stern Test With Mega Cap Earnings On Deck - 2023-01-30: "Tech stocks have fallen pretty far down on the list of concerns (and the price action) is telling us something," said Bank of America strategists ahead of a key week for mega cap earnings., Author: Martin Baccardax, Source: The Street, Sentiment Score: 0.14012
-20. PodcastGuests.com, a Thriving Membership Platform Connecting Podcasters with Great Guests, Announces Acquisition - 2023-01-30: PodcastGuests.com, a Thriving Membership Platform Connecting ... PR ..., Author: FE International, Source: PR Newswire, Sentiment Score: 0.384029
-21. PodcastGuests.com, a Thriving Membership Platform Connecting Podcasters with Great Guests, Announces Acquisition - 2023-01-30: FE International, Inc., the global market leader in mid-market technology mergers and acquisitions ( M&amp;A ) , announces the acquisition of membership platform PodcastGuests.com by serial entrepreneur Brian Scully., Author: PRNewswire, Source: Benzinga, Sentiment Score: 0.367499
-22. WISeKey Launches eTreeNFT.com Connecting Trees, NFTs and Crypto on a Unique Opportunity for Creating New and Totally Sustainable Asset-Based Markets for Sequestering CO2 - 2023-01-30: WISeKey Launches eTreeNFT.com Connecting Trees, NFTs and Crypto on a Unique Opportunity for Creating New and Totally SustainableAsset-Based Markets for Sequestering ..., Author: Wisekey International Holding SA, Source: GlobeNewswire, Sentiment Score: 0.244448
-23. One Way For F-1 Foreign Students To Get Green Cards - 2023-01-30: A popular path for foreign students to get a U.S. green card is: F-1 student visa -&gt; Optional Practical Training (OPT) post graduate employment authorization -&gt; H1B work visa -&gt; Labor certification and I-140 sponsorship by an employer. The road's not easy, but here's an explanation of how it's ..., Author: Andy J. Semotiuk, Source: Forbes, Sentiment Score: 0.169725
-24. After Layoffs And A CEO Swap, Cometeer's Frozen Coffee Pod Business Is In Hot Water - 2023-01-30: In December, Cometeer quietly conducted layoffs and installed its chief operating officer as co-CEO. Former employees spoke of dysfunction and high executive turnover as growth has slowed at the most-funded coffee startup ever, where headcount is down nearly 50%., Author: Alex Konrad, Source: Forbes, Sentiment Score: 0.014385
-25. An Uncomfortable Bill Gates Tries to Explain His Jeffrey Epstein Dinners - 2023-01-30: The billionaire was put on the spot yet again., Author: Colette Bennett, Source: The Street, Sentiment Score: -0.084522
-26. Congress to grill TikTok on list of concerns from spying to child safety - .com - 2023-01-30: Congress to grill TikTok on list of concerns from spying to child safety UPI News ..., Author: Unknown Author, Source: UPI Business, Sentiment Score: -0.100933
-27. Spanish Company Kognia Explains How It's Shaping Tactical Analysis In Soccer - 2023-01-30: In such a monied industry, state-the-art soccer analysis tools have the potential to impact the game significantly., Author: Henry Flynn, Source: Forbes, Sentiment Score: 0.152575
-28. 1 Potentially Explosive Warren Buffett Stock Down 62% to Buy - 2023-01-30: Snowflake is an unusual Buffett-backed stock that could crush the market over the next decade., Author: Keith Noonan, Source: Motley Fool, Sentiment Score: 0.284815
-29. Despite Elon Musks Warnings, AI Is Here and Growing Fast - 2023-01-30: Billionaire Elon Musk has long been a skeptic of the development of artificial intelligence ( AI ) - despite being one of its biggest proponents. Not only is Musk a founding member of OpenAI, creator of ChatGPT, but his Tesla and other companies he's created are also at the forefront of the ..., Author: Caleb Naysmith, Source: Benzinga, Sentiment Score: 0.110937
-30. Accela Senior Vice President of Marketing Heidi Lorenzen Named an APPEALIE 2022 SaaS Marketing Leader Award Winner - 2023-01-30: Accela Senior Vice President of Marketing Heidi Lorenzen Named ... PR ..., Author: Accela, Source: PR Newswire, Sentiment Score: 0.510008
-31. Will Strong Data Center Growth Aid AMD's Q4 Earnings Growth? - 2023-01-30: Advanced Micro Devices' (AMD) fourth-quarter 2022 earnings are expected to have been affected by weak PC shipments, offset by robust demand for data center solutions., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.207758
-32. ChatGPT Is the New Disruptor-in-Chief But There's a Catch - 2023-01-30: The new AI tool has the potential to disrupt almost every profession, say two experts who also warn of its dangers., Author: Luc Olinga, Source: The Street, Sentiment Score: 0.187024
-33. Chess.com Or ChatGPT? Both Sites Are Failing To Keep Up With Demand - 2023-01-30: ChatGPT has taken the tech world by storm throughout the past few months, impressing engineers, coders and investors alike. ChatGPT, the AI-powered search engine run by OpenAI, surpassed 10 million users in less than 40 days., Author: Aaron Bry, Source: Benzinga, Sentiment Score: 0.079319
-34. The US consumer is starting to freak out - 2023-01-30: The engine of the U.S. economy-consumer spending-is starting to sputter. Retail purchases have fallen in three of the past four months. Spending on services, including rent, haircuts and the bulk of bills, was flat in December, after adjusting for inflation, the worst monthly reading in nearly a ..., Author: Unknown Author, Source: Fox Business News, Sentiment Score: -0.072722
-35. Western Digital Likely For Sharp Revenue Decline Taking Cue From Seagate, Intel &amp; Microsoft, Analyst Says - 2023-01-30: Credit Suisse analyst Shannon Cross reiterated Neutral on Western Digital Corp WDC with a $42 price target. Western Digital will likely report 2Q23 results after the market on Jan. 31, 2023., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: -0.243575
-36. Bill Gates Has Big Plans for the Future of Healthcare - From an HIV Vaccine to Eradicating Malaria, Here's How the Billionaire Is Reshaping Healthcare - 2023-01-30: Bill Gates rose to prominence during the internet's early growth stages and the dot-com boom. His company, Microsoft Corp. MSFT, became a big player in the tech scene in the early 1980s and launched its initial public offering ( IPO ) in 1986., Author: Caleb Naysmith, Source: Benzinga, Sentiment Score: 0.288454
+1. Asia shares brace for rate hikes, earnings rush - 2023-01-30: SYDNEY, Jan 30 ( Reuters ) - Asian shares started cautiously on Monday in a week that is certain to see interest rates rise in Europe and the United States, along with U.S. jobs and wage data that may influence how much further they still have to go., Author: Wayne Cole, Source: Reuters, Sentiment Score: 0.007225
+2. Why This May Be A Life-Changing Rally; Futures Fall - 2023-01-30: Why This May Be A Life-Changing Rally. Futures Fall Investor's Business Daily ..., Author: ED CARSON, Source: Investors Business Daily, Sentiment Score: 0.162936
+3. Apple's 2023 High-End iPhone 15 Series May Have These 2 Major Updates; Analyst Expects Android Vendors To Ape Changed Design - 2023-01-30: Apple Inc. AAPL is likely to make some significant changes to its iPhone 15 series, slated for a 2023 launch., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.16524
+4. Bitcoin, Ethereum, Dogecoin Spike Amid Risk-On Rebound - 2023-01-30: Major coins traded in the green on Sunday evening, as the global market cap rose 1.34% to $1.08 trillion, as of 8:30 p.m. EST. What Happened: The largest cryptocurrency by market value Bitcoin BTC/USD traded above $23,000. Ethereum ETH/USD was changing hands at $1,567, up 1.70% in the last 24 ..., Author: Mehab Qureshi, Source: Benzinga, Sentiment Score: 0.106651
+5. False iPhone Crash Detection Alerts Flood Japan - 2023-01-30: False Apple Inc AAPL iPhone 14 "Crash Detection" alerts are now troubling emergency responders near skiing areas in Japan. What Happened: Japanese fire departments near skiing areas are facing an influx in emergency calls as iPhone 14 models triggered false crash detection alerts, reported Apple ..., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: -0.476524
+6. Amid S&amp;P 500's Rebound, Analyst Recommends Paring Back Positions: 'Breakout Is Going To Fool Most People' - 2023-01-30: The stock market has gotten off to a strong start in 2023, a welcome development following the dismal showing the previous year. The S&amp;P 500 Index, a broader market gauge, fell about 19.5% in 2022 but has gained over 6% since then., Author: Shanthi Rexaline, Source: Benzinga, Sentiment Score: -0.062262
+7. Amazon, Alphabet, Apple, Intel and Microsoft are part of Zacks Earnings Preview - 2023-01-30: Chicago, IL - January 30, 2023 - Zacks.com releases the list of companies likely to issue earnings surprises. This week's list includes Amazon ( AMZN Quick QuoteAMZN - ) , Alphabet ( GOOGL Quick QuoteGOOGL - ) , Apple ( AAPL Quick QuoteAAPL - ) , Intel ( INTC Quick QuoteINTC - ) and Microsoft ( ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.002391
+8. Stocks Lower, Big Tech Earnings, Fed Rate Decision, Adani Group, Eagles &amp; Chiefs - Five Things To Know - 2023-01-30: Stock futures lower as markets face headline risk gauntlet. Week Ahead: Fed decision, big tech earnings, jobs in focus. Adani group hits back at Hindenburg short report. Renault and Nissan overhaul alliance, putting carmakers on equal terms and Philadelphia eagles favored over Kansas City Chiefs ..., Author: Martin Baccardax, Source: The Street, Sentiment Score: 0.071775
+9. Nearly 43% of Warren Buffett's Portfolio Is Invested in These 5 Tech Stocks - 2023-01-30: Should these stocks make up a big chunk of your portfolio, too?, Author: Keith Speights, Source: Motley Fool, Sentiment Score: 0.222689
+10. Dow futures drop 200 points as Fed decision, tech earnings await - 2023-01-30: U.S. stock futures slumped on Monday to kick off a big week that features a Federal Reserve interest-rate decision, a jobs report and several key technology-sector earnings., Author: Steve Goldstein, Source: MarketWatch, Sentiment Score: 0.012311
+11. Will Apple Follow Tech Peers In Announcing A Mass Layoff This Week? Analyst Says iPhone Maker In A 'Unique' Position - 2023-01-30: Apple Inc. AAPL would lead the week's big tech earnings news flow, with the company scheduled to report on Thursday after the close. No Massive Layoffs: The most widely seen tech theme of recent times - massive layoffs - may be absent from Apple's scheme of things, analyst Daniel Ives said in a ..., Author: Shanthi Rexaline, Source: Benzinga, Sentiment Score: 0.047713
+12. Should Invesco FTSE RAFI US 1000 ETF  ( PRF )  Be on Your Investing Radar? - 2023-01-30: Style Box ETF report for PRF ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.229009
+13. Nasdaq leads drop in futures ahead of Fed rate decision - 2023-01-30: Jan 30 ( Reuters ) - Nasdaq led declines in U.S. futures on Monday, dropping more than 1%, with growth stocks falling at the start of a week packed with central bank rate decisions and earnings from several high-profile companies. The U.S., Author: Reuters, Source: Reuters, Sentiment Score: 0.038229
+14. Apple Supplier Jabil Starts Making AirPods Components In India, Reduce Dependence On China - 2023-01-30: Key Apple Inc AAPL supplier Jabil Inc JBL has begun making components for AirPods in India, making way for the partial manufacture of Apple's second product after iPhone. Jabil's Indian division has started shipping AirPods enclosures, or plastic bodies, to China and Vietnam, where Apple ..., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: 0.130621
+15. Time to short Goldilocks? Why this major bank's strategist is now turning cautious. - 2023-01-30: Any investor out there who isn't nervous, perhaps should recheck his gut, says our call of the day, from Standard Chartered's global head of research, Eric Robertsen., Author: Barbara Kollmeyer, Source: MarketWatch, Sentiment Score: -0.065532
+16. Big Tech's squeeze of technology innovators is costing you more for apps and other internet services - 2023-01-30: Change intellectual property law to help level the playing field or risk America's global tech leadership., Author: Mike Feibus, Source: MarketWatch, Sentiment Score: 0.188588
+17. Elon Musk Gets Sound Advice, Trump Hits Campaign Trail, ChatGPT Faces China Threat And More: 5 Key Stories You May Have Missed From The Weekend - 2023-01-30: The phrase "lull before the storm" could best characterize the weekend as market participants prepped for a rough week in the wake of the Fed meeting and the impending tech earnings. Here's a recap of a few major headlines that hit the wire over the weekend: 1. Apple MR Headset A Hit Or Flop?, Author: Shanthi Rexaline, Source: Benzinga, Sentiment Score: 0.021854
+18. Think Chevron's Profit Was Obscene? 5 Companies Will Blow It Away - 2023-01-30: Chevron's ( CVX ) giant $36.5 billion 2022 profit certainly turned heads - including at the White House. But plenty of S&amp;P 500 companies will make even more than the oil giant. The bulk of S&amp;P 500 companies this week will report their fourth-quarter and full 2022 results., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.31514
+19. Google Stock: YouTube Expected To Be Drag On Earnings Amid Apple, TikTok Woes - 2023-01-30: Google Stock: YouTube Expected To Be Drag On Earnings Amid ... Investor's Business Daily ..., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.045557
+20. Tech Futures Sell Off With Fed Meeting In Sight - 2023-01-30: Dow Jones Futures Fall With Fed Meeting In Sight. Tesla Stock ... Investor's Business Daily ..., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.200889
+21. Stock Market Today: Stocks Lower Ahead of Fed, 'Tech Super Bowl', And Jobs Data Week - 2023-01-30: Tech stocks, riding their best start to the year since 2001, face a series of tests this week in the form of mega-cap earnings, a Fed rate decision and January jobs data., Author: Martin Baccardax, Source: The Street, Sentiment Score: 0.002409
+22. Meta Quest Pro Now Available For A Discount Of $400: Worth It? - 2023-01-30: Meta Platforms Inc.'s META most recent VR device Meta Quest Pro is now available at a discounted price on Amazon.com AMZN - but still it might be expensive for some consumers. What Happened: Three months after its launch, Meta Quest Pro is available for $1,110 on Amazon., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.18027
+23. Elon Musk Finds These 8 iPhone Notes Features 'Useful' - 2023-01-30: Apple Inc.'s AAPL iPhone 13 might be the most popular smartphone sold in the U.S. as of April 2022, but do all iPhone users know how to use the Notes app available on the device to its full potential? Sadly No., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.265523
+24. Apple 'Fake' News Alert: iOS 17 Stories Pushed By Troll Account - 2023-01-30: An Apple Inc. AAPL watcher has warned people against believing any stories about iOS 17 citing a "troll account." What Happened: Mark Gurman took to Twitter to warn his 283.9K followers that news reports citing a "troll account known to make up fake information" have circulated updates about ..., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.141326
+25. Shares and bonds markets worldwide nervy as rate-hike week looms - 2023-01-30: Stock markets worldwide halted their January rally on Monday, pausing for breath at the start of an agenda-setting week of central bank rate hikes and data releases ..., Author: Reuters, Source: Business Standard, Sentiment Score: -0.133101
+26. Why These Analysts Are Warning Investors January Stock Market Rally 'Will Not Last' - 2023-01-30: The SPDR S&amp;P 500 ETF Trust SPY is off to a strong start to 2023, and investors are hopeful that the stock market's 2022 struggles are now fully in the rearview mirror. Unfortunately, multiple market analysts are warning investors not to chase the recent market rally., Author: Wayne Duggan, Source: Benzinga, Sentiment Score: 0.109713
+27. Big Week Ahead for Q4 Earnings, Econ Data - 2023-01-30: Following another solid week of gains -- which is sizing up to be one of the strongest January trading months in years -- pre-market futures are selling off some., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.105746
+28. Wall Street Waits for Fed FOMC and Key Economic Data - 2023-01-30: We have a consequential week in the markets ahead of us - perhaps the most consequential week we've seen so far this year. Not only do we have a new Fed funds rate out mid-week ( expectations are for a 25 bps bump to a 4.50-4.75% range ) , but we also get roughly 20% of the S&amp;P 500 reporting ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.108188
+29. The Unbelievable Story Of The 'Pokémon Go Grandpa,' The 74-Year-Old Cycling Around With 64 Devices Attached To His Bicycle - 2023-01-30: When one thinks of an average gamer, the image that comes to mind is not usually that of an elderly person. Nor is it a person who plays with 64 devices at the same time. And, least of all, someone who uses all those mobile phones to play while cycling around the city., Author: Franca Quarneti, Source: Benzinga, Sentiment Score: 0.147337
+30. Apple Music launches Rihanna's Road to Halftime ahead of Super Bowl LVII - Investing News Network - 2023-01-30: Apple Music launches Rihanna's Road to Halftime ahead of Super Bowl LVII Investing News Network ..., Author: Unknown Author, Source: Investing News Network, Sentiment Score: 0.355853
+31. Stock Market DownAhead Of Fed Meeting; Chinese Internet Stock Drops; - 2023-01-30: Stock Market Down Ahead Of Fed Meeting. Nvidia Sells Off ... Investor's Business Daily ..., Author: KIMBERLEY KOENIG, Source: Investors Business Daily, Sentiment Score: 0.021624
+32. Dollar Weakness, Easing Of Supply Constraints Likely To Add To Better Margins For Apple, Analyst Says - 2023-01-30: Credit Suisse analyst Shannon Cross reiterated Outperform on Apple Inc AAPL with a $184 price target. Apple will report F1Q23 results after the market on February 2. The analyst maintained her quarter estimates, including revenue of $121.6 billion and EPS of $1.92, which she lowered on December ..., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: 0.100432
+33. Spotify Likely For Upside From Gross Profit Leverage, Pricing Power From Music Subscriptions, Analyst Says - 2023-01-30: Benchmark analyst Mark Zgutowicz maintained Spotify Technology SA SPOT with a Buy and raised the price target from $125 to $130 in front of SPOT's 4Q report. The consensus' 23E expectations understate Premium and Ad-supported gross profit leverage following '22's "trough" podcast profitability., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: 0.064869
+34. Meta Needs To Slash Another 7.5K Jobs To Accommodate Metaverse Ambitions, Analyst Says - 2023-01-30: Benchmark analyst Mark Zgutowicz remained Hold-rated on Meta Platforms Inc META before Meta's 4Q report. The analyst did not see enough '23 opex leverage to spark the stock price in a weak ad spend environment and lingering ROAS impact from Apple Inc AAPL ATT., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: 0.02882
+35. Apple May Soon Be Next to Bet on Foldable Tech - 2023-01-30: With Lenovo and LG already selling foldable tablets, rumors of a similar iPad abound., Author: Veronika Bondarenko, Source: The Street, Sentiment Score: 0.171495
+36. Super Bowl LVII: When is it? Where is it? And how much are tickets? - 2023-01-30: Here's everything you need to know ahead of the biggest U.S. sporting event of the year., Author: Weston Blasi, Source: MarketWatch, Sentiment Score: 0.331815
 37. Volatility Test: VIX Makes an Early Move Higher as Stocks Slide Ahead of Manic Market Week - 2023-01-30: ( Monday Market Open ) For those who like market news, this week has no shortage. There's something for everyone with central bank meetings, earnings, and a jobs report all straight ahead. Monday kicked off with heavy selling before the open., Author: Shawn Cruz, Source: Benzinga, Sentiment Score: 0.00717
 38. Bitcoin aims for $25K as institutional demand increases and economic data soothes investor fears - 2023-01-30: Strong corporate earnings and investors' anticipation of a Federal Reserve pivot are helping to cement the case for risk assets like Bitcoin., Author: Unknown Author, Source: Cointelegraph, Sentiment Score: 0.075825
-39. "Rule Breaker Investing" -- Talking About Stocks, Staying Hydrated, and Other Life Things - 2023-01-30: Another mailbag full of great questions and comments from listeners., Author: Motley Fool Staff, Source: Motley Fool, Sentiment Score: 0.278288
-40. Corporate Burnout Is Coming For Investor Profits - 2023-01-30: The more companies lose to corporate burnout, the less profit they have to show investors., Author: Q.ai - Powering a Personal Wealth Movement, Source: Forbes, Sentiment Score: -0.124928
-41. Bill Gates Responds To Jeffrey Epstein Ties For 'Over Hundredth Time': 'I Shouldn't Have Had Dinners With Him' - 2023-01-30: Microsoft co-founder and former CEO Bill Gates has repeatedly said he regrets ever interacting with convicted sex offender Jeffrey Epstein. In a new interview on ABC Australia's 7.30, a current affairs program, he downplayed his ties to the financier, who reportedly died by suicide in jail in 2019., Author: Adam Eckert, Source: Benzinga, Sentiment Score: -0.215201
-42. The number of 'millionaire renters' has tripled --- here are the cities where they're most likely to live - 2023-01-30: The typical 'millionaire renter' is a millennial who rents a three-bedroom, according to RentCafe., Author: Aarthi Swaminathan, Source: MarketWatch, Sentiment Score: 0.14433
-43. Top Stock Picks for Week of January 30, 2023 - 2023-01-30: A Financial and Ecommerce Company for Your Review., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.229586
-44. More than 75,000 tech-sector employees have lost their jobs since the start of the year - 2023-01-30: Tens of thousands of tech employees have been laid off so far in 2023, according to data compiled by Layoffs.fyi., Author: James Rogers, Source: MarketWatch, Sentiment Score: -0.096463
-45. Futures: Fed Meeting, Big Earnings On Deck; What To Do Now - 2023-01-30: Futures: Fed Meeting, Big Earnings On Deck. What To Do Now Investor's Business Daily ..., Author: SCOTT LEHTONEN, Source: Investors Business Daily, Sentiment Score: 0.137108
-46. Russian millionaire on trial in hack, insider trade scheme - 2023-01-30: BOSTON ( AP ) - A wealthy Russian businessman and associates made tens of millions of dollars by cheating the stock market in an elaborate scheme that involved hacking into U.S. computer networks to steal insider information about companies such as Microsoft and Tesla, a prosecutor told jurors ..., Author: Unknown Author, Source: Associated Press, Sentiment Score: -0.099634
-47. Cloud is Growing 20% Annually: 3 Tech Stocks to Buy for Exposure - 2023-01-30: The global cloud computing market is valued at $369 billion and expected to grow 15% annually to $1.6 trillion by ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.118161
-48. The race of the AI labs heats up - 2023-01-30: ChatGPT is not the only game in town ..., Author: Unknown Author, Source: The Economist, Sentiment Score: 0.181139
-49. Time to Take Another Bite of Apple Before Q1 Earnings? - 2023-01-30: Apple has managed to deliver better-than-expected results despite facing a challenging business environment, exceeding the Zacks Consensus EPS Estimate in four consecutive quarters. Can the streak continue?, Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.105668
-50. What Investors Need to Know About the Latest News From Microsoft - 2023-01-30: We've also got insight on Alphabet, Kimberly-Clark, and Big Lots., Author: Dylan Lewis, Source: Motley Fool, Sentiment Score: 0.062167
+39. The 'return of the DOJ' hangs over Google as online ads decline - 2023-01-30: The very thing that has Google entangled in a handful of government lawsuits - its dominance of the digital-ad market - is the dominant story line when it reports fiscal fourth-quarter results Thursday., Author: Jon Swartz, Source: MarketWatch, Sentiment Score: -0.105602
+40. What stock-market investors need to know as busiest week of earnings season begins - 2023-01-30: U.S. companies are in a precarious spot as the most important week of earnings season begins Monday., Author: Joseph Adinolfi, Source: MarketWatch, Sentiment Score: -0.021722
+41. Apple earnings may rely on an unlikely hero amid iPhone uncertainty - 2023-01-30: Apple Inc.'s Mac business has enjoyed a renaissance that's lasted far beyond the initial pandemic-driven boom. Can the momentum continue?, Author: Emily Bary, Source: MarketWatch, Sentiment Score: 0.014542
+42. Stock Market Today: Stocks Slump Ahead of Tech Earnings, Fed Meeting - 2023-01-30: Stock Market Today: Stocks Slump Ahead of Tech Earnings, Fed ... Kiplinger's Personal Finance ..., Author: Karee Venema, Source: Kiplinger, Sentiment Score: 0.264165
+43. Fasten your seatbelts - 2023-01-30: Fasten your ..., Author: Stephen Culp, Source: Reuters, Sentiment Score: 0.016913
+44. Futures: Fed Meeting, Big Earnings On Deck; What To Do Now - 2023-01-30: Futures: Fed Meeting, Big Earnings On Deck. What To Do Now Investor's Business Daily ..., Author: SCOTT LEHTONEN, Source: Investors Business Daily, Sentiment Score: 0.137108
+45. Time to Take Another Bite of Apple Before Q1 Earnings? - 2023-01-30: Apple has managed to deliver better-than-expected results despite facing a challenging business environment, exceeding the Zacks Consensus EPS Estimate in four consecutive quarters. Can the streak continue?, Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.105668
+46. Apple execs violated labor law after remarks that interfered with organizing: report - 2023-01-30: U.S. labor lawyers reportedly found that Apple Inc. executives ran afoul of labor law, after they made remarks and set rules that chilled efforts to organize., Author: Bill Peters, Source: MarketWatch, Sentiment Score: -0.264894
 Stock Closing Prices for Past 3 Months (Fridays):
-2022-11-11: 100.7900, 2022-11-18: 94.1400, 2022-11-25: 93.4100, 2022-12-02: 94.1300, 2022-12-09: 89.0900, 2022-12-16: 87.8600, 2022-12-23: 85.2500, 2022-12-30: 84.0000, 2023-01-06: 86.0800, 2023-01-13: 98.1200, 2023-01-20: 97.2500, 2023-01-27: 102.2400, </t>
+2022-11-11: 148.6829, 2022-11-18: 150.2621, 2022-11-25: 147.1037, 2022-12-02: 146.8057, 2022-12-09: 141.1941, 2022-12-16: 133.5961, 2022-12-23: 130.9641, 2022-12-30: 129.0472, 2023-01-06: 128.7393, 2023-01-13: 133.8444, 2023-01-20: 136.9333, 2023-01-27: 144.9385, </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Predicted Stock Closing Prices for Next 12 Weeks (Fridays):
-2023-02-10: 97.6100, 2023-02-17: 97.2000, 2023-02-24: 93.5000, 2023-03-03: 94.9000, 2023-03-10: 90.7300, 2023-03-17: 98.9500, 2023-03-24: 98.1300, 2023-03-31: 103.2900, 2023-04-14: 102.5100, 2023-04-21: 106.9600, 2023-04-28: 105.4500, 
-Predicted Market Sentiment: 0.14389325999999997</t>
+2023-02-10: 150.2124, 2023-02-17: 151.7443, 2023-02-24: 145.9351, 2023-03-03: 150.2323, 2023-03-10: 147.7157, 2023-03-17: 154.1814, 2023-03-24: 159.4036, 2023-03-31: 164.0291, 2023-04-14: 164.3374, 2023-04-21: 164.1484, 2023-04-28: 168.7838, 
+Predicted Market Sentiment: 0.07817373913043481</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-01-27</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Week Ending on 2023-01-27:
+News Summary:
+1. Earnings Watch: Microsoft, Tesla and Intel are about to face the doubters - 2023-01-23: Tesla, Intel and Microsoft face bigger questions about the path forward, after their shares took a beating last year., Author: Bill Peters, Source: MarketWatch, Sentiment Score: -0.029223
+2. Apple targets raising India production share to up to 25%: Piyush Goyal - 2023-01-23: Apple Inc wants India to account for up to 25% of its production from about 5%-7% now, the trade minister told a conference on Monday., Author: Unknown Author, Source: Money Control, Sentiment Score: 0.062624
+3. Apple's Top Execs Sold Stock in a Volatile 2022, but CEO Tim Cook Held Off - 2023-01-23: Apple Execs Sold Stock in a Volatile 2022, but CEO Tim Cook Held Off ..., Author: Ed Lin, Source: Barrons, Sentiment Score: 0.062206
+4. Apple targeting to raise India production share to 25%: Piyush Goyal - 2023-01-23: NEW DELHI ( Reuters ) - Apple Inc wants India to account for up to 25% of its production from about 5%-7% now, the trade minister told a conference on Monday. "Apple, another success story," Piyush Goyal said. "They are already at about 5-7% of their manufacturing in India., Author: Reuters, Source: Business Standard, Sentiment Score: 0.181243
+5. Will Apple Stock Beat the Market in 2023? - 2023-01-23: After a slide in the second half of 2022, here's what it will take for Apple to bounce back., Author: Jeremy Bowman, Source: Motley Fool, Sentiment Score: 0.046115
+6. Why Warren Buffett Wants Apple Stock to Tumble - 2023-01-23: Is the legendary investor being irrational? Not at all., Author: Keith Speights, Source: Motley Fool, Sentiment Score: 0.196913
+7. How Will iPhone 15 Pro Differ From Basic Model? - 2023-01-23: Apple Inc's AAPL iPhone 15 series may have the same display sizes as its predecessors, but there are other updates, especially concerning iPhone 15 high-end models, that may catch users' attention., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.185502
+8. Nervous About the Stock Market? 1 ETF to Keep Your Money Safer - 2023-01-23: If the market falls further, this ETF can help protect your savings., Author: Katie Brockman, Source: Motley Fool, Sentiment Score: 0.082649
+9. Is John Hancock Multifactor Large Cap ETF  ( JHML )  a Strong ETF Right Now? - 2023-01-23: Smart Beta ETF report for ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.199536
+10. Nasdaq Off To Best Start Since 2019; These Stocks Are Leading - 2023-01-23: Nasdaq Off To Its Best Start Since 2019. These Stocks Are Leading Investor's Business Daily ..., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: -0.019369
+11. Apple Anticipates India Production Share To Rise 25% In Attempt To Diversify Base Beyond China - 2023-01-23: Apple Inc AAPL wants India to be responsible for up to 25% of its production from the present 5%-7%, the trade minister recounted. Minister Piyush Goyal emphasized Apple launching the most recent models from India, manufactured in India, Reuters reports., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: 0.16832
+12. Apple Avoids Layoffs, Dogecoin Surges, South America's Common Currency Move And More: 5 Key Stories You May Have Missed From The Weekend - 2023-01-23: As the fourth-quarter reporting season starts in earnest this week, chatter over the weekend focused on its impact on the fledgling recovery seen in the market. Discussions also centered around the odds of a recession materializing and the likely monetary policy stance of the Federal Reserve when ..., Author: Shanthi Rexaline, Source: Benzinga, Sentiment Score: -0.026623
+13. Skechers To Rally 40%? Here Are 10 Other Analyst Forecasts For Monday - 2023-01-23: Credit Suisse raised the price target for Exelon Corporation EXC from $42 to $46. Credit Suisse analyst Nicholas Campanella maintained an Outperform rating. Exelon shares fell 0.1% to $42.32 in pre-market trading. Goldman Sachs boosted the price target for Ally Financial Inc. ALLY from $28 to $36., Author: Lisa Levin, Source: Benzinga, Sentiment Score: 0.179668
+14. Tech Shows Initial Signs of Revival: Trend Likely to Continue - 2023-01-23: Technology behemoths like AAPL, MSFT, META, GOOGL and NVDA are currently trading at huge discount from their respective 52-week high levels., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.087205
+15. Futures Rise Ahead Of Key Economic Data, Earnings Reports - 2023-01-23: Dow Jones futures rose Monday ahead of a busy week of key economic data and as the dollar dropped to an eight-month low. A big week of earnings news includes results from Tesla, due out Wednesday. Advanced Micro Devices ( AMD ) jumped more than 2% after a Barclays upgrade to overweight., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.210354
+16. Investors Are Betting on Tech Again - 2023-01-23: Tech stocks rose significantly in the last trading recession, and for good reason., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.322652
+17. Warren Buffett Just Beat the S&amp;P 500 by the Widest Margin Since 2007. Can He Do It Again in 2023? - 2023-01-23: Berkshire Hathaway's strategy worked to perfection in 2022., Author: Daniel Foelber, Source: Motley Fool, Sentiment Score: 0.162422
+18. Is Most-Watched Stock Apple Inc.  ( AAPL )  Worth Betting on Now? - 2023-01-23: Zacks.com users have recently been watching Apple (AAPL) quite a bit. Thus, it is worth knowing the facts that could determine the stock's prospects., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.246348
+19. Apple 14-inch MacBook Pro Review  ( 2023 ) : Extreme Performance In a Great Build - 2023-01-23: The latest 14-inch MacBook Pro sticks with an excellent build, but speeds things up with the M2 Pro chip., Author: Jacob Krol, Source: The Street, Sentiment Score: 0.315048
+20. Want to Get Richer? 3 Stocks to Buy in 2023 and Hold Forever - 2023-01-23: These companies are titans of their industries, likely to provide consistent gains over the long term., Author: Dani Cook, Source: Motley Fool, Sentiment Score: 0.248986
+21. ChatGPT Is Just the Beginning - AI Is Quietly Reshaping Every Aspect of Your Life - 2023-01-23: ChatGPT became a viral sensation upon its release to the public on Nov. 30, 2022. It hit over 1 million users in under a week and has only continued to grow, with hundreds of companies using its application programming interface ( API ) integrations to create or improve their products., Author: Caleb Naysmith, Source: Benzinga, Sentiment Score: 0.204601
+22. Market on Tipping Point of New Bull Trend: These 5 Charts Illustrate Why - 2023-01-23: You never really know when a new bull trend has arrived for sure. However, by looking at different sides of the market you can begin to put the pieces of the puzzle together., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: -0.064631
+23. iPhone 4 Bursts Into Flames In Ohio Family's House - 2023-01-23: An Apple Inc. AAPL iPhone burst into flames while a couple and their five kids slept in the house. What Happened: Brian Leisgang, who resides in Ohio with his wife and their five children, slept through the night, unaware that an iPhone 4 had burst inside his house and caused a fire, reported ..., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: -0.1684
+24. Publishers Clearing House Records Significant Quarter-Over-Quarter User Growth on Comscore - 2023-01-23: NEW YORK, Jan. 23, 2023 ( GLOBE NEWSWIRE ) -- Publishers Clearing House ( PCH ) , a leading digital entertainment and commerce destination for millions of US consumers, today announced that the company recorded a traffic lift of 13.6% from Q3 2022 to Q4 2022, reaching an audience of 15,683,000 ..., Author: Globe Newswire, Source: Benzinga, Sentiment Score: 0.331937
+25. Why Buying This FAANG Stock Could Be a Genius Move - 2023-01-23: This company stands out among its fast-growing tech rivals., Author: Matthew DiLallo, Source: Motley Fool, Sentiment Score: 0.318104
+26. Apple Leads The Market Higher After Recently Lagging: Here's What's Happening - 2023-01-23: Apple, Inc AAPL was popping up over 1% on Monday, leading the S&amp;P 500 slightly higher. The tech giant has lagged the broad market index during the last two most recent rebounds, unlike during the last short-term bully cycle, which took place between June 17 and Aug. 17., Author: Melanie Schaffer, Source: Benzinga, Sentiment Score: 0.129423
+27. Big Tech Reports: Global Week Ahead - 2023-01-23: Microsoft (MSFT), the second biggest U.S. company by market value, reports on Tuesday, followed by Elon Musk's Tesla (TSLA) on Wednesday. That's just the warm up for next week., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: -0.024076
+28. SPY: SPY Jumps Above 200 Day Moving Average, Getting Bulls Excited - 2023-01-23: SPY: SPY Jumps Above 200 Day Moving Average, Getting Bulls ... ..., Author: Unknown Author, Source: Stocknews.com, Sentiment Score: 0.210437
+29. Stock Market Recovery: These 4 Stocks Have Been on the Rise in 2023 - 2023-01-23: These companies' shares sank in 2022, but investors are feeling more bullish about them in 2023., Author: Dani Cook, Source: Motley Fool, Sentiment Score: 0.19781
+30. Why Apple  ( AAPL )  is Poised to Beat Earnings Estimates Again - 2023-01-23: Apple (AAPL) has an impressive earnings surprise history and currently possesses the right combination of the two key ingredients for a likely beat in its next quarterly report., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.319265
+31. Warren Buffett Ditched His Flip Phone for an iPhone in 2020 and Drinks 5 Cans of Coke a Day - That's What Makes Him One of the Greatest Investors of All Time - 2023-01-23: Business magnate Warren Buffett is widely regarded as one of the greatest investors of the modern-day world. His seemingly unmatched and consistent value-investing strategies have earned him the title of Oracle of Omaha., Author: Caleb Naysmith, Source: Benzinga, Sentiment Score: 0.292927
+32. MATANA Is Back: Which Stocks to Buy Now - 2023-01-23: Many investors are still unconvinced that technology stocks have already bottomed, adding fuel to the bullish case., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.004831
+33. World's First ETF Turns 30, Here's How Much Money You'd Have If You Invested $1,000 When It Launched - 2023-01-23: The SPDR S&amp;P 500 ETF Trust SPY, the first U.S.-based exchange-traded fund, was launched 30 years ago this week. In the past three decades, State Street's so-called "Spider" fund has grown to become the world's largest ETF and one of the most popular ways for investors to make diversified bets on ..., Author: Wayne Duggan, Source: Benzinga, Sentiment Score: 0.278697
+34. Stocks Make a Quiet Move Upward Ahead of Thursday's GDP, 'Pause' Talk - 2023-01-23: ( Monday Market Open ) This week and next could go a long way toward determining how the current quarter plays out on Wall Street. Between now and February 4, we'll receive earnings reports from close to half of S&amp;P 500® companies, including 90 this seek., Author: TD Ameritrade Network, Source: Benzinga, Sentiment Score: 0.059872
+35. Stocks Make a Quiet Move Upward Ahead of Thursday's GDP, 'Pause' Talk - 2023-01-23: ( Monday Market Open ) This week and next could go a long way toward determining how the current quarter plays out on Wall Street. Between now and February 4, we'll receive earnings reports from close to half of S&amp;P 500® companies, including 90 this seek., Author: Shawn Cruz, Source: Benzinga, Sentiment Score: 0.059872
+36. The big banks want to take on PayPal in e-commerce, but that's harder than it seems - 2023-01-23: PayPal helped make it easy for consumers to store their payment information for online purchases. Now the banks want in on that game ..., Author: Emily Bary, Source: MarketWatch, Sentiment Score: -0.009669
+37. Stock Market Gains As Weak Economic Reading Fuels Rate Hopes; Tech-Heavy Nasdaq Leads - 2023-01-23: Stock Market Gains As Weak Economic Reading Fuels Rate Hopes ... Investor's Business Daily ..., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.057512
+38. Stock Market Erases Some Gains; Weak Economic Data Fuels Rate Hopes; Tech-Heavy Nasdaq Leads - 2023-01-23: Stock Market Gains As Weak Economic Reading Fuels Rate Hopes ... Investor's Business Daily ..., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.043237
+39. Etsy, IBD Stock Of The Day, Jumps Past An Early Entry Point - 2023-01-23: Etsy Stock Emerges From A Difficult Time Investor's Business Daily ..., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.171782
+40. Wells Fargo And Other Banks Join Forces To Tap $2T Payments App Market Against Apple Pay, PayPal - 2023-01-23: Wells Fargo &amp; Co WFC, Bank Of America Corp BAC, JP Morgan Chase &amp; Co JPM, and four other banks worked on a digital wallet linked to their debit and credit cards. Early Warning Services LLC would manage the wallet that aimed to compete with Apple Inc AAPL Apple Pay, and PayPal Holdings, Inc PYPL, ..., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: -0.067388
+41. Why Apple Stock Was Climbing Today - 2023-01-23: Analysts expect the company to beat estimates in its upcoming earnings report., Author: Jeremy Bowman, Source: Motley Fool, Sentiment Score: 0.033316
+42. Here's what Apple's mixed-reality headset could feature - 2023-01-23: Apple Inc. is expected to take on Meta Platforms Inc. with the launch of a mixed-reality headset later this year., Author: Emily Bary, Source: MarketWatch, Sentiment Score: 0.127949
+43. Tesla Stock Is on a Tear. Watch for This Level as Short Sellers Get Burned. - 2023-01-23: Short sellers have been covering some bearish bets on Tesla stock as the shares have gained in 2023. Tesla stock is flying as short sellers scramble to close out bets that the price would fall. Investors should watch a key level when asking themselves how long can the run will continue., Author: Al Root, Source: Barrons, Sentiment Score: 0.181033
+44. Amazon Earnings Set to Disappoint: Time to Buy AMZN Stock at a Steep Discount? - 2023-01-23: With a slowdown in online spending, and inflation raising its transportation and fulfillment costs, Amazon is dealing with some painful headwinds in the ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.109407
+45. Futures: Stocks Extend Gains; 10 Stocks To Buy And Watch - 2023-01-23: Dow Jones Rallies 250 Points. What To Do Now. 10 Best Stocks To ... Investor's Business Daily ..., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.195698
+46. Bitcoin Prices Retain Bulk Of Gains After Climbing To 5-Month High - 2023-01-23: Bitcoin prices have shown strength lately, holding on to most of their recent upside after rising to their loftiest value in over five months. The digital currency has been rising lately in spite of industry headwinds, including the FTX collapse and Genesis Capital declaring bankruptcy., Author: Charles Bovaird, Source: Forbes, Sentiment Score: 0.172904
+47. How Often Are Dividends Paid &amp; When Do You Get Them? - 2023-01-23: Knowing when, and how, you'll get paid is important., Author: Jason Hall, Source: Motley Fool, Sentiment Score: 0.178626
+48. 'It is an employer's market': Tech layoffs may have turned the Great Resignation into the Great Recommitment - 2023-01-23: The flood of recently laid-off tech workers on the job market has upended the dynamic between employers and employees, leading to prolonged job searches., Author: Jon Swartz, Source: MarketWatch, Sentiment Score: 0.038379
+49. Tesla Bull Says Time For Tim Cook To Step Down: Apple In 'Serious Trouble' If Elon Musk's Company Begins Making Phones - 2023-01-24: Apple, Inc. AAPL CEO Tim Cook and Elon Musk may have patched up following the latter's outburst over the tech giant pulling out most of its ads from Twitter - but a Tesla bull in late November lashed out at the Apple chief over the way he was leading the company., Author: Shanthi Rexaline, Source: Benzinga, Sentiment Score: 0.10569
+50. Big Tech Layoffs; Signs of Trouble in the Housing Market - 2023-01-24: Alphabet and Microsoft are laying off a combined 22,000 employees. Is Apple next?, Author: Chris Hill, Source: Motley Fool, Sentiment Score: 0.10954
+51. Apple Gives 10-Year-Old iPhone Model An iOS Update - 2023-01-24: Apple Inc. AAPL continues to update older devices, going back to the iPhone 5s. Here's a complete list of models that have received a software update., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.108681
+52. Markets Turn More Bullish Ahead Of Earnings - 2023-01-24: The CNN Money Fear and Greed index showed improvement in overall market sentiment among US investors. US stocks closed higher ahead of a busy week of earnings. Markets are expecting the US Federal Reserve to increase rates by 25 basis points at its upcoming meeting. Shares of Tesla, Inc., Author: Lisa Levin, Source: Benzinga, Sentiment Score: -0.147285
+53. Investors Await Tech Earnings in Next Test for Markets - 2023-01-24: Disappointment could leave the broader market vulnerable to a selloff following tech stocks' strong start to the year., Author: Charley Grant, Source: Wall Street Journal, Sentiment Score: -0.034419
+54. Nasdaq Rises Over 2%, Volatility In Markets Decreases - 2023-01-24: US stocks closed higher on Monday amid surge in technology stocks. All three major indices extended Friday's gains, with the tech-laden Nasdaq index leading the rally. The US Federal Reserve is widely expected to increase rates by 25 basis points at its February 1 policy announcement., Author: Lisa Levin, Source: Benzinga, Sentiment Score: 0.109269
+55. Is WisdomTree U.S. Quality Dividend Growth ETF  ( DGRW )  a Strong ETF Right Now? - 2023-01-24: Smart Beta ETF report for ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.306165
+56. Should WisdomTree U.S. LargeCap ETF  ( EPS )  Be on Your Investing Radar? - 2023-01-24: Style Box ETF report for ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.221918
+57. 1 Warren Buffett Stock to Buy in 2023 and Hold Forever - 2023-01-24: This company's stock has risen over 400% since Buffett bought it in 2016., Author: Dani Cook, Source: Motley Fool, Sentiment Score: 0.3342
+58. Apple Weighs Content Deals With Disney, Other Partners For VR Headset - 2023-01-24: Apple Inc AAPL discussed developing VR content for the platform with about half a dozen media partners, including Walt Disney Co DIS and Dolby Laboratories Inc. Apple worked on updating its own Apple TV+ material to work with the headset, Bloomberg reports., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: 0.170687
+59. Amazon Introduces Affordable Healthcare Subscription Service For Uninsured Consumers - 2023-01-24: Amazon.Com, Inc AMZN launched RxPass in select U.S. states, a new Prime membership benefit from Amazon Pharmacy that provides patients with affordable access to generic medications that treat more than 80 common health conditions for just $5 a month., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: 0.263413
+60. Tech earnings could wreck Wall Street's party | Business - 2023-01-24: Tech earnings could wreck Wall Street's party CNN International ..., Author: Nicole Goodkind, Source: CNN, Sentiment Score: 0.069805
+61. Tech earnings could wreck Wall Street's party | Business - 2023-01-24: Tech earnings could wreck Wall Street's party ..., Author: Nicole Goodkind, Source: CNN, Sentiment Score: 0.069805
+62. Intel Faces Heat From Arm's Growing Popularity With Cloud Computing Giants Like Amazon and Microsoft - 2023-01-24: Softbank Group Corp SFTBF SFTBY Arm-based chips won market share in PCs and rivaled Intel Corp INTC in the increasingly crucial data-center market., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: 0.061806
+63. Microsoft, Alphabet Cry Poor Right Before Making $32.8 Billion - 2023-01-24: Layoff announcements from Microsoft ( MSFT ) and Alphabet ( GOOGL ) , along with their tumbling stock prices, make it seem like giant tech S&amp;P 500 companies are in dire straits. But they're on the verge of making billions - in just one quarter., Author: MATT KRANTZ, Source: Investors Business Daily, Sentiment Score: 0.050602
+64. Futures Down: Economic Data Due; 6 Earnings Reporters - 2023-01-24: Dow Jones Futures Fall As 6 Key Earnings Movers Report. Microsoft ... Investor's Business Daily ..., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.162977
+65. Apple Headset OS' Internal Name 'xrOS' Filed For Trademark By Mysterious Shell Company - 2023-01-24: Apple Inc.'s AAPL internal name for its mixed reality, or MR, headset's operating system continues to get filed globally by a shell company. What Happened: In December, it was reported that Apple engineers were using both "realityOS" and "xrOS" names for its MR headset's operating system internally., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: -0.035108
+66. How to Find Strong Computer and Technology Stocks Slated for Positive Earnings Surprises - 2023-01-24: Investors looking for ways to find stocks that are set to beat quarterly earnings estimates should check out the Zacks Earnings ESP., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.355444
+67. Timing the Market: EPS is a Lagging Indicator - 2023-01-24: The S&amp;P 500 Index's price has bottomed prior to its earnings in the past 3 bear markets. Today, Andrew Rocco unveils some forward looking indicators investors can focus on., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.083326
+68. 'We don't want to work for jerks': The impact of bad bosses, gaslighting and toxic workplaces on your mental health.  ( It's like being in a dysfunctional marriage. )  - 2023-01-24: When managers are more open about their own mental health journey, experts say it can help create a more inclusive and supportive environment., Author: Quentin Fottrell, Source: MarketWatch, Sentiment Score: 0.092225
+69. Will Meta Platforms Be a Trillion-Dollar Stock by 2030? - 2023-01-24: This former member of the 12-zero club isn't down for the count yet., Author: Leo Sun, Source: Motley Fool, Sentiment Score: 0.090773
+70. Jim Cramer's top 10 things to watch in the market Tuesday: Club earnings, AMD downgrade, Disney hope - 2023-01-24: Big day of earnings for Club holdings as the Dow, S&amp;P 500 and Nasdaq look to open lower after back-to-back gains., Author: Jim Cramer, Source: CNBC, Sentiment Score: 0.077626
+71. Top Stories Tuesday, Jan. 24 - 2023-01-24: Former President Donald Trump has reportedly hired trial lawyer Joe Tacopina in a matter about alleged defamatory statements made by the former criminal division chief at the U.S. attorney's office in Manhattan, Mark Pomerantz., Author: Vandana Singh, Source: Benzinga, Sentiment Score: 0.163204
+72. The Zacks Analyst Blog Highlights Microsoft, Tesla, Apple and Alphabet - 2023-01-24: Microsoft, Tesla, Apple and Alphabet are part of the Zacks top Analyst Blog., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: -0.077095
+73. Stock Market News for Jan 24, 2023 - 2023-01-24: U.S. stocks closed higher on Monday, led by a tech rally, as investors geared up for a busy week of earnings and grew optimistic about the Fed going slow on its interest rate hikes in the coming months., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.25251
+74. The Zacks Analyst Blog Highlights Apple, Microsoft, Meta Platforms, Alphabet and NVIDIA - 2023-01-24: Apple, Microsoft, Meta Platforms, Alphabet and NVIDIA are part of the Zacks top Analyst Blog., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.084623
+75. America's biggest banks are taking on Apple Pay and PayPal | Business - 2023-01-24: America's biggest banks are taking on Apple Pay and PayPal CNN International ..., Author: Chris Isidore, Source: CNN, Sentiment Score: -0.14679
+76. America's biggest banks are taking on Apple Pay and PayPal | Business - 2023-01-24: America's biggest banks are taking on Apple Pay and PayPal CNN International ..., Author: Chris Isidore, Source: CNN, Sentiment Score: -0.14679
+77. ChatGPT Is Doing for AI What Apple's iPhone Did for Smartphones - 2023-01-24: The first iPhone came out in June 2007, and now 84% of Americans own a smartphone and many can't imagine a world without them. While Apple Inc. AAPL didn't make the first smartphone, it was the device that catapulted the technology to its modern-day success, quickly selling millions of units and ..., Author: Caleb Naysmith, Source: Benzinga, Sentiment Score: 0.053857
+78. The Zacks Analyst Blog Highlights Apple, Alphabet, NVIDIA, Microsoft and Meta Platforms - 2023-01-24: Apple, Alphabet, NVIDIA, Microsoft and Meta Platforms are part of the Zacks top Analyst Blog., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.304614
+79. Apple is making a move for Premier League U.K. rights - 2023-01-24: Apple reportedly has its sights on the world's biggest soccer league., Author: Owen Poindexter, Source: MarketWatch, Sentiment Score: 0.250981
+80. What's in Store for Big Tech ETFs in Q4 Earnings? - 2023-01-24: The technology sector, which was hit the hardest by soaring yields and a hawkish Fed, showed a strong comeback to start 2023., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.130474
+81. Facebook App, Messenger Slated For Updates - 2023-01-24: Meta Platforms Inc.'s META Facebook application and Messenger may get a few updates, which might make your experience on the platform more convenient. What Happened: Social media expert Ahmed Ghanem took to Twitter to share a new feature that Facebook is testing to add to the app footer on Apple ..., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.135669
+82. Viral TikTok: Multitasking On Your iPhone Be Tedious No More - 2023-01-24: Multitasking on your Apple Inc. AAPL devices including iPhones can become tiresome at times. Whether you're flipping between a text message and deciding what food to order for delivery or watching your favorite TV show while running errands, here's how you can multitask like a pro., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.146501
+83. Apple builds on privacy commitment by unveiling new education and awareness efforts on Data Privacy Day - 2023-01-24: In celebration of Data Privacy Day, Apple® today unveiled a new set of educational resources designed to help users take control of their data. This press release features multimedia. View the full release here: https://www.businesswire.com/news/home/20230124005418/en/, Author: Unknown Author, Source: Investing News Network, Sentiment Score: 0.256766
+84. S&amp;P 500 ETFs in Focus as SPY Turns 30 - 2023-01-24: We highlight the ETF that revolutionized investing &amp; 3 cheaper alternatives ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.291297
+85. Apple Headed for Down Sales Year in Fiscal 2023, Bernstein Analyst Contends - 2023-01-24: With sales softening for iPhones, Macs and iPads, Apple could be headed for a year-over-year revenue decline for the fiscal year ending in September. That's according to Bernstein analyst Toni Sacconaghi, who remains lukewarm on the prospects for Apple ( ticker: AAPL ) shares., Author: Eric J. Savitz, Source: Barrons, Sentiment Score: -0.031654
+86. 2 No-Brainer Growth Stocks to Buy in 2023 - 2023-01-24: These stocks have enjoyed triple-digit growth in the last five years, with 2023 a major buying opportunity., Author: Dani Cook, Source: Motley Fool, Sentiment Score: 0.346091
+87. Start of Earnings Traffic Jam Delivers Mixed Results as Market Waits for Microsoft - 2023-01-24: The fun starts today after the closing bell with Microsoft MSFT and Texas Instruments TXN. Then get ready for IBM IBM after tomorrow's close and Intel INTC the day after. There's a little concern about what MSFT might report, and that could be one factor pushing stock index futures lower this ..., Author: TD Ameritrade Network, Source: Benzinga, Sentiment Score: 0.045897
+88. Can Netflix Win A Best Picture Like Apple? Will Big Box Office Movies Have Their Day In The Awards Spotlight Again? 2 Big Questions From The Academy Award Nominations - 2023-01-24: On Tuesday, the nominations for the 95th Academy Awards were announced. Several critical darlings received numerous nominations and many of the top nominated movies from the recent Golden Globes awards show also heard their names called again. The 95th Academy Awards will air on ABC on March 12., Author: Chris Katje, Source: Benzinga, Sentiment Score: 0.557634
+89. How Spotify's Downsizing Could Affect You - 2023-01-24: The music streamer takes a step back from its major investments amid layoffs ..., Author: Danni Button, Source: The Street, Sentiment Score: 0.058322
+90. Futures Fall On MSFT Guidance; Earnings Wave Continues - 2023-01-24: Futures Rise As MSFT Earnings 'Azure' Investors. Tesla On Tap Investor's Business Daily ..., Author: ED CARSON, Source: Investors Business Daily, Sentiment Score: 0.024369
+91. MSFT, Boeing Hit Futures; Tesla Due As Earnings Wave Continues - 2023-01-24: Futures Rise As MSFT Earnings 'Azure' Investors. Tesla On Tap Investor's Business Daily ..., Author: ED CARSON, Source: Investors Business Daily, Sentiment Score: 0.009787
+92. Apple  ( AAPL )  Gains As Market Dips: What You Should Know - 2023-01-24: Apple (AAPL) closed at $142.53 in the latest trading session, marking a +1.01% move from the prior day., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.168289
+93. Futures Turn Lower On MSFT Guidance After Market Holds Strong - 2023-01-24: Dow Jones Futures: Microsoft Erases Gains On Weak Guidance ... Investor's Business Daily ..., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.036483
+94. Better Buy in 2023: Apple Stock vs. Disney Stock - 2023-01-25: One of these stocks has risen more than 670% in the last decade., Author: Dani Cook, Source: Motley Fool, Sentiment Score: 0.25539
+95. Satya Nadella Touts Microsoft's ChatGPT Advantage: 'Age Of AI' - 2023-01-25: Microsoft Corporation MSFT CEO Satya Nadella, while sharing the earning results for the latest quarter, hailed the developments in the field of artificial intelligence and the tech giant's role in "powering it.", Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.235514
+96. 3 No-Brainer Warren Buffett Stocks to Buy Right Now - 2023-01-25: Investors can set their portfolios up for long-term growth with these Buffett stocks., Author: Harsh Chauhan, Source: Motley Fool, Sentiment Score: 0.40353
+97. Apple Launched 1st Mach 39 Years Ago: Do You Find It Still Cool? - 2023-01-25: Former Apple Inc. AAPL CEO Steve Jobs created history 39 years ago on this day when he launched the first-ever Macintosh at $2,495 - a steal at the time. What Happened: The Macintosh project was started by Jef Raskin in the late 1970s., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.136521
+98. Should iShares Core S&amp;P 500 ETF  ( IVV )  Be on Your Investing Radar? - 2023-01-25: Style Box ETF report for ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.200408
+99. Better Buy: Apple Stock vs. Netflix Stock - 2023-01-25: These companies' stocks have been on the rise in 2023., Author: Dani Cook, Source: Motley Fool, Sentiment Score: 0.163778
+100. Apple's Chip Strategy Is Great News for Shareholders, Bad News for Skyworks, Broadcom, and Qualcomm - 2023-01-25: The tech giant's chip design ambitions are yielding dividends, literally and figuratively., Author: Billy Duberstein, Source: Motley Fool, Sentiment Score: 0.108698
+101. Will Soft Processor Revenues Hurt Intel  ( INTC )  Q4 Earnings? - 2023-01-25: Intel (INTC) is likely to have recorded lower revenues from the CCG segment due to challenging macroeconomic conditions and cheaper alternatives from rival firms., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.085409
+102. Will Lower Data Center Revenues Dent Intel  ( INTC )  Q4 Earnings? - 2023-01-25: Intel (INTC) is likely to have recorded lower revenues from the DCAI segment due to dwindling PC sales, supply chain adversities and an</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Predicted Stock Closing Prices for Next 12 Weeks (Fridays):
+2023-02-03: 153.4503, 2023-02-10: 150.2124, 2023-02-17: 151.7443, 2023-02-24: 145.9351, 2023-03-03: 150.2323, 2023-03-10: 147.7157, 2023-03-17: 154.1814, 2023-03-24: 159.4036, 2023-03-31: 164.0291, 2023-04-14: 164.3374, 2023-04-21: 164.1484, 
+Predicted Market Sentiment: 0.13089129569892477</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-01-20</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Week Ending on 2023-01-20:
+News Summary:
+1. Tech's slump masks rally sweeping across S&amp;P 500 - 2023-01-16: While the benchmark is down 17% from its record high set on Jan. 3, 2022, about three-quarters of the stocks in the index are up 20% or more from their 52-week lows, according to data compiled by Bloomberg., Author: Unknown Author, Source: Money Control, Sentiment Score: 0.045808
+2. Davos draws record crowds, but its relevance is fading | Business - 2023-01-16: Davos draws record crowds, but its relevance is fading ..., Author: Julia Horowitz, Source: CNN, Sentiment Score: -0.046013
+3. Should iShares S&amp;P 100 ETF  ( OEF )  Be on Your Investing Radar? - 2023-01-16: Style Box ETF report for ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.135953
+4. History Says the Nasdaq Could Soar in 2023 -- 5 Stocks You'll Wish You'd Bought if It Does - 2023-01-16: The Nasdaq-100 tends to bounce back strongly in the year after a loss., Author: Anthony Di Pizio, Source: Motley Fool, Sentiment Score: 0.151687
+5. Zacks Value Trader Highlights: Berkshire Hathaway, Apple, Bank of America, Chevron, The Coca-Cola - 2023-01-16: Berkshire Hathaway, Apple, Bank of America, Chevron, The Coca-Cola are part of the Zacks Value Trader blog., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.284122
+6. Tim Cook Reacts As Apple Watch Saves Life Of Indian Teen Who Fell Into 150-Feet Valley - 2023-01-16: Apple Inc.'s AAPL Watch Series 7 has worked as a miracle to save a teenager's life in India after he slipped 130 to 150 feet into a valley. What Happened: Smit Metha, a 17-year-old teenager from India, was on a hike when he slipped and fell into a valley and misplaced his iPhone., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.147465
+7. The Zacks Analyst Blog Highlights Lenovo Group, HP, Dell Technologies and Apple - 2023-01-16: Lenovo Group, HP, Dell Technologies and Apple are part of the Zacks top Analyst Blog., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: -0.230213
+8. Warren Buffett Owns a Lot of Stocks -- Here's the One I'm Most Excited About - 2023-01-16: Interest rates could continue rising in 2023. This stock should benefit., Author: Justin Pope, Source: Motley Fool, Sentiment Score: 0.1864
+9. E-book market size to grow by USD 6.93 billion from 2021 to 2026: A descriptive analysis of customer landscape, vendor assessment, and market dynamics - Technavio - 2023-01-16: E-book market size to grow by USD 6.93 billion from 2021 to 2026: A ... PR ..., Author: Technavio, Source: PR Newswire, Sentiment Score: 0.320994
+10. Is TSMC Stock a Buy Now? - 2023-01-16: The world's largest chipmaker still has plenty of room to grow., Author: Leo Sun, Source: Motley Fool, Sentiment Score: 0.057229
+11. 3 Tech Stocks Approved by Warren Buffett - 2023-01-16: The Oracle of Omaha's company has really warmed up to tech stocks over the last decade., Author: Keith Noonan, Source: Motley Fool, Sentiment Score: 0.29553
+12. 2 Top Tech Stocks to Buy for the Long Haul - 2023-01-16: A market correction is the perfect time to buy formerly high-flying growth stocks., Author: Rich Duprey, Source: Motley Fool, Sentiment Score: 0.19036
+13. 2 Tech ETFs to Help You Capture the Sector's Rebound - 2023-01-16: Tech did not perform well in 2023, but investors are starting to feel more optimistic., Author: Bram Berkowitz, Source: Motley Fool, Sentiment Score: 0.082373
+14. Did Someone Say Dividends? Here's How Much Of These Tech Stocks You Need To Yield $100 Per Month - 2023-01-16: The S&amp;P 500 dropped 19.2% in 2022, its worst performance in any year since it declined 38.4% during the global financial crisis in 2008. The Dow Jones Industrial Average finished 2022 down 8.5% on the year, while the Nasdaq declined 33%., Author: AJ Fabino, Source: Benzinga, Sentiment Score: -0.163785
+15. Better Growth Stock in 2023: Apple vs. AMD - 2023-01-16: Apple and AMD suffered stock declines in 2022, but that hasn't dampened their excellent long-term outlooks., Author: Dani Cook, Source: Motley Fool, Sentiment Score: 0.2851
+16. 2 FAANG Stocks to Buy in 2023 and 1 to Avoid: Here's Why - 2023-01-16: Discover why two FAANG stocks are poised to bounce back in 2023 and beat the market with their current spring-loaded share price discounts, while another looks like a questionable idea today., Author: Anders Bylund, Source: Motley Fool, Sentiment Score: 0.146883
+17. Ryan Cohen Takes Stake In Alibaba, Nudges Buyback Boost - 2023-01-17: Activist investor Ryan Cohen has reportedly acquired a stake in Chinese e-commerce giant Alibaba Group Holding Ltd. BABA worth hundreds of millions of dollars and is privately nudging the company to hasten its share-repurchase program., Author: Bhavik Nair, Source: Benzinga, Sentiment Score: 0.258147
+18. Apple Leaker Hints At Surprise Announcement Today - 2023-01-17: Apple Inc. AAPL is gearing to make an unexpected announcement on Tuesday, according to a prominent leaker. Could it be about MacBook Pros or the highly-anticipated mixed-reality headset?, Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.145405
+19. Foxconn's new iPhone business chief helped meet Apple's high standards - 2023-01-17: The Taiwanese firm named Michael Chiang as head of its iPhone assembly operations as it seeks to elevate younger executives to maintain supply chain leadership., Author: Bloomberg, Source: South China Morning Post, Sentiment Score: 0.075971
+20. Microsoft Will Top Apple, Google, Thanks To ChatGPT: Expert - 2023-01-17: Microsoft Corporation MSFT will soon add OpenAI's artificial intelligence, or AI chatbot, chatGPT, to its cloud-based Azure services, setting the stage for what looks like a dominant year for the tech giant., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.161687
+21. Did Amazon Just Overpay for 'Thursday Night Football'? - 2023-01-17: Viewership in the first season of the deal fell short of expectations., Author: Jeremy Bowman, Source: Motley Fool, Sentiment Score: 0.028596
+22. Warren Buffett Is Raking in $4.84 Billion in Annual Dividend Income From These 6 Stocks - 2023-01-17: These half-dozen stocks will account for the lion's share of Berkshire Hathaway's more than $6 billion in dividend income this year., Author: Sean Williams, Source: Motley Fool, Sentiment Score: 0.272984
+23. CBOE Volatility Index Settles At One-Year Low As Banks Kick Off Quarterly Earnings Season - 2023-01-17: US stocks closed higher on Friday, with the S&amp;P 500 and Nasdaq closing at their strongest levels in a month, as banks kicked off the quarterly earnings season. JPMorgan Chase &amp; Co JPM and Bank of America Corp BAC reported better-than-expected earnings for the latest quarter on Friday., Author: Lisa Levin, Source: Benzinga, Sentiment Score: 0.081521
+24. 3 Great Foreign Companies to Invest In Right Now - 2023-01-17: Think U.S. stocks are cheap? These overseas gems are absolute bargains., Author: Billy Duberstein, Source: Motley Fool, Sentiment Score: 0.236022
+25. Should Vanguard Mega Cap Growth ETF  ( MGK )  Be on Your Investing Radar? - 2023-01-17: Style Box ETF report for ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.27753
+26. China's Pandemic Pain, Apple 'Surprise' Rumors, Summers Backing Of IRS And More: 5 Key Stories You May Have Missed From The Weekend - 2023-01-17: The long weekend saw analysts and investors mulling over the past week's strong run-up and establishing patterns to predict the future trajectory. Cryptocurrencies saw some upward bounce over the weekend, reigniting hopes of a resurgence after the disappointing performances in 2022., Author: Shanthi Rexaline, Source: Benzinga, Sentiment Score: 0.063449
+27. Futures Drop Ahead Of Manufacturing, Inflation Data - 2023-01-17: Dow Jones futures dropped Tuesday morning ahead of New York regional manufacturing data, and another round of key inflation numbers due out Wednesday. Fourth-quarter earnings season continues Tuesday, with results from Dow Jones stock Goldman Sachs ( GS ) and Morgan Stanley ( MS ) ., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.172933
+28. Apple unveils M2 Pro and M2 Max: next-generation chips for next-level workflows - Investing News Network - 2023-01-17: Apple unveils M2 Pro and M2 Max: next-generation chips for next-level workflows Investing News Network ..., Author: Unknown Author, Source: Investing News Network, Sentiment Score: 0.383496
+29. Apple unveils MacBook Pro featuring M2 Pro and M2 Max, with more game-changing performance and the longest battery life ever in a Mac - 2023-01-17: New MacBook Pro features up to 6x faster performance than fastest Intel-based MacBook Pro and support for up to 96GB of unified memory for demanding pro workflows, Author: Unknown Author, Source: Investing News Network, Sentiment Score: 0.360703
+30. Apple introduces new Mac mini with M2 and M2 Pro - more powerful, capable, and versatile than ever - 2023-01-17: Starting at just $599, Mac mini is even more affordable Apple® today unveiled the new Mac mini®, supercharged by M2 and the all-new M2 Pro. With the M2 chip, Mac mini is even more powerful, capable, and affordable with a new starting price of just $599., Author: Unknown Author, Source: Investing News Network, Sentiment Score: 0.310133
+31. Apple Watch Saves Woman's Life By Identifying Heart Block - 2023-01-17: A 59-year-old Apple Inc. AAPL user said Apple Watch saved her life after it alerted her about an irregular rhythm. What Happened: Elaine Thompson from Gateshead, England said that she consulted a doctor when Apple Watch alerted her about an unidentified heart condition, reported Independent., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.202851
+32. Selects: Top stories this evening - 2023-01-17: Our specially curated package of the most interesting articles to help you stay at the top of your game., Author: Unknown Author, Source: Money Control, Sentiment Score: 0.080906
+33. Apple launches faster MacBook Pro laptops with new custom chips - 2023-01-17: Apple Inc. is upgrading its MacBook Pro laptop to feature faster chips, the consumer-electronics giant announced Tuesday ..., Author: Emily Bary, Source: MarketWatch, Sentiment Score: 0.336714
+34. FAANG Stocks Look Ready to Soar Later This Month. Here's Why. - 2023-01-17: Currency headwinds are fading faster than expected., Author: Jeremy Bowman, Source: Motley Fool, Sentiment Score: 0.03637
+35. Will Warren Buffett Own a Virtual Reality Stock in 2023? - 2023-01-17: A rumored new device could catapult Apple into the virtual reality space., Author: Jeff Santoro, Source: Motley Fool, Sentiment Score: 0.298671
+36. Starbucks Taps Online Ordering Market Via iOS, Android Devices By Extending Collaboration With DoorDash - 2023-01-17: Starbucks Corp SBUX and DoorDash, Inc DASH expanded their partnership with a new delivery service launching on Jan. 17, 2023, in Northern California, Texas, Georgia, Florida, and other select markets., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: 0.274563
+37. Apple Site Crashes Before 2 New Products Dropped - What Buyers Need to Know - 2023-01-17: The new Apple products have been long-awaited, and some folks may have to wait even longer now., Author: Jena Greene, Source: The Street, Sentiment Score: 0.07387
+38. Buy Apple and IBM Stock Ahead of Earnings, Says Analyst - 2023-01-17: With tech earnings season now dead ahead, investors are tweaking their portfolios ahead of what could be a tumultuous period for the group, with the Street anticipating generally weak guidance for 2023 amid ongoing concerns about a potential recession. But it's not going to be a complete wipeout., Author: Eric J. Savitz, Source: Barrons, Sentiment Score: -0.102186
+39. Your Clothes Are Getting Smarter - The $60 Billion Wearables Market Is Producing Some of the Most Revolutionary and Bizarre Technology of the Decade - 2023-01-17: Wearable technology is becoming an integral part of everyday life, but it's been hit or miss Alphabet Inc. GOOGL released Google Glass in 2013, which faded into obscurity almost as soon as it was released. Google ultimately lost more than $895 million from the product, and the future of the ..., Author: Caleb Naysmith, Source: Benzinga, Sentiment Score: 0.266525
+40. Apple AirTags and Bluetooth Trackers Are Officially a Billion-Dollar Industry - Here's What To Know, Trends, and the Best Ways To Invest - 2023-01-17: Apple Inc.'s AAPL AirTag might not seem like a big-ticket item, but the company has now sold over $1 billion worth - or about 55 million - of the handy little trackers since launching in April 2021., Author: Caleb Naysmith, Source: Benzinga, Sentiment Score: 0.147191
+41. Everything You Need to Know About the M2 Mac Mini and MacBook Pros - 2023-01-17: The new Mac Mini as well as the 14-inch and 16-inch MacBook Pros feature the M2, M2 Pro, or M2 Max processors., Author: Jacob Krol, Source: The Street, Sentiment Score: 0.355841
+42. Apple Stock: Here's How Much Upside May Be Left After Recent Rally - 2023-01-17: Apple made news and the stock followed with a big rally. Here's how the charts look now., Author: Bret Kenwell, Source: The Street, Sentiment Score: 0.007347
+43. Apple Just Dropped a Bunch of New Products - Here's What's Coming - 2023-01-17: Faster speeds and processing power never looked so good., Author: Veronika Bondarenko, Source: The Street, Sentiment Score: 0.239965
+44. Home and Away: Bank of Japan, China Data, Davos Distract From Bank Earnings as Yields Rise, Stocks Retreat - 2023-01-17: ( Tuesday Market Open ) Following Friday's mixed earnings performance from four of the largest U.S. banks, Tuesday kicked off with more mixed results from two closely followed names in investment banking. That, along with overnight weakness in Europe and Asia, helped set a negative tone in the ..., Author: Shawn Cruz, Source: Benzinga, Sentiment Score: 0.01922
+45. 'When I Find Things I Have A Lot Of Conviction In, I Go All-in': Ryan Cohen's Stake In Alibaba And History Of Activism - 2023-01-17: Activist investor Ryan Cohen has made a name for himself for investments in several companies that became popular with retail traders, including GameStop Corp GME and Bed Bath &amp; Beyond BBBY. Now, a new holding by Cohen has been announced. Here's a look at his new stake and the past history of his ..., Author: Chris Katje, Source: Benzinga, Sentiment Score: 0.106318
+46. 8 Cheap Tech Stocks to Watch in 2023 - 2023-01-17: These stocks can be considered a deal in the technology sector. Find out if these cheap tech stocks are right for you., Author: Nicholas Rossolillo, Source: Motley Fool, Sentiment Score: 0.279497
+47. Supreme Court asks U.S. government to weigh in on Apple patent dispute - 2023-01-17: The Supreme Court has asked the Biden administration to weigh in on a billion-dollar intellectual property case brought by the California Institute of Technology against Apple Inc. and Broadcom Inc., Author: Jan Wolfe, Source: MarketWatch, Sentiment Score: 0.252836
+48. Apple  ( AAPL )  Gains As Market Dips: What You Should Know - 2023-01-17: Apple (AAPL) closed at $135.94 in the latest trading session, marking a +0.88% move from the prior day., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.169875
+49. John Chambers expects a 'tough' 2023 but plenty of opportunities for AI, cybersecurity - 2023-01-17: "This year is going to be tough," Chambers told MarketWatch. "However, I believe strongly that downturns are when the next generation of leaders can emerge." ..., Author: Jon Swartz, Source: MarketWatch, Sentiment Score: -0.00727
+50. The 5 tech earnings to watch as holiday-season results start to flood in - 2023-01-17: After one of the worst years for tech stocks in recent memory, tech companies are about to detail exactly how good -- or, more likely, how bad -- their holiday seasons were., Author: Therese Poletti, Source: MarketWatch, Sentiment Score: 0.074583
+51. Apple will delay AR glasses, focus instead on cheaper mixed-reality headset: report - 2023-01-18: Apple Inc. is expected to release its first mixed-reality headset later this year, but the release of its follow-up product, augmented-reality glasses, has been postponed, according to a new report., Author: Mike Murphy, Source: MarketWatch, Sentiment Score: -0.035245
+52. Apple Effect? Decentraland  ( MANA )  Soars 73% In A Week - 2023-01-18: Mana MANA/USD, the native token of the metaverse game Decentraland, skyrocketed by 73% over the past week, although it is currently trading flat at $0.70., Author: Mehab Qureshi, Source: Benzinga, Sentiment Score: 0.124038
+53. Apple Plans Cheaper MR Headset For Wider Market - 2023-01-18: Apple Inc.'s AAPL highly-anticipated first mixed reality headset will launch this year, but the augmented reality glasses might not release anytime soon. What Happened: Apple has postponed its plans to launch AR glasses as a follow-up product after the release of its first MR headset, reported ..., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.058854
+54. Apple's Faster Chips Alone Can Boost Mac Growth: Munster - 2023-01-18: Apple, Inc. AAPL on Tuesday kicked off its launch event for the year with the unveiling of the M2 Pro and M2 Pro Max chips that would be made available for the MacBook Pro and Mac Mini., Author: Shanthi Rexaline, Source: Benzinga, Sentiment Score: 0.304358
+55. Taiwan Q4 GDP unexpectedly shrinks, worst performance in 13 years - 2023-01-18: TAIPEI, Jan 18 ( Reuters ) - Taiwan's trade-dependent economy unexpectedly contracted in the fourth quarter, putting in its worst performance in 13 years, hit by a drop in exports on slowing global tech demand and COVID-related chaos in its largest market China., Author: Reuters, Source: Reuters, Sentiment Score: -0.226668
+56. Apple's Chinese Suppliers Win Expansion Permits In India As iPhone-Maker Attempts To Reduce Dependence On China - 2023-01-18: More than a dozen Apple Inc's AAPL Chinese suppliers won initial clearance from India to expand as the iPhone maker strived to diversify its assembly network beyond China. About 14 suppliers bagged permits from India after Apple promoted the need for their growing presence in India, Bloomberg ..., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: 0.133899
+57. 3 Rock-Solid Dividend Stocks to Buy in 2023 - 2023-01-18: You can rest easy while owning these dependable cash generators., Author: Joe Tenebruso, Source: Motley Fool, Sentiment Score: 0.384366
+58. In a Stunning Move, Apple Plans to Ditch Highly Valued Wireless Component Suppliers - 2023-01-18: This personal electronics device company pursues expensive, complex initiatives to improve its competitive positioning., Author: Rob Starks Jr, Source: Motley Fool, Sentiment Score: 0.133555
+59. Opinion: After the recession, a new dynamism will emerge - 2023-01-18: The future is bright, and four years from now we will feel better no matter who is in the White House., Author: Peter Morici, Source: MarketWatch, Sentiment Score: -0.251755
+60. Is Invesco FTSE RAFI US 1000 ETF  ( PRF )  a Strong ETF Right Now? - 2023-01-18: Smart Beta ETF report for PRF ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.277579
+61. Should Vanguard Russell 1000 Growth ETF  ( VONG )  Be on Your Investing Radar? - 2023-01-18: Style Box ETF report for VONG ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.256053
+62. 3 Stocks to Buy if They Take a Dip - 2023-01-18: You never want to pay too much for a stock. Aim to buy when it's undervalued., Author: Selena Maranjian, Source: Motley Fool, Sentiment Score: 0.282249
+63. Apple Is Taking on Meta in Virtual Reality. It's Not Going to Be Easy. - 2023-01-18: This year is set to finally see the launch of Apple 's mixed-reality headset. It's looking to take market share from Meta the current leader in the space, but product delays and finding a price point which will convince consumers to switch are problems., Author: Adam Clark, Source: Barrons, Sentiment Score: 0.0
+64. YouTube Beats Apple, Spotify As Top Podcast Platform Choice - 2023-01-18: Not Apple Inc. AAPL or Spotify Technology S.A. SPOT, one out of three listeners prefer Alphabet Inc.'s GOOG GOOGL YouTube for listening to podcasts. What Happened: The latest survey by Morning Consult suggests that 33% of U.S. adults prefer YouTube as their chosen podcast platform, followed by ..., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.152913
+65. Bill Gates Opts For Samsung Over Apple As 'Daily Driver' Phone - 2023-01-18: Ever wondered which smartphone Microsoft Corporation co-founder Bill Gates uses? Well, wonder no longer. We have the answer for you. What Happened: In an "Ask Me Anything" session on Reddit, Gates revealed that he has Samsung Electronics Co, Ltd SSNLF Galaxy Z Fold 4., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.102477
+66. Viral TikTok: Can Anyone Really See Where You've Been With Just A Little iPhone Trick? - 2023-01-18: Did you know Apple Inc.'s AAPL smartphones can track users' whereabouts, but could it be visible to anyone using someone else's iPhone without adequate privacy layers?, Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.014343
+67. Wearable Payment Device Market will value USD 436.0 billion by 2030 : GreyViews - 2023-01-18: Pune India, Jan. 18, 2023 ( GLOBE NEWSWIRE ) -- The market has been studied for the below mentioned-segmentation and regional analysis for North America, Europe, Asia, South America, and the Middle East and Africa. These are the key regions where the wearable payment device market is operating ..., Author: Globe Newswire, Source: Benzinga, Sentiment Score: 0.222758
+68. Tesla Has the Most Valuable Car Brand, but It Isn't the Strongest - 2023-01-18: Tesla 's brand is the most valuable among the world's auto makers, but it could be stronger. Tesla investors, along with Wall Street, are worried that CEO Elon Musk's ownership of Twitter is hurting Tesla's brand image. Recently, BrandFinance ranked the top 500 global brands by value., Author: Al Root, Source: Barrons, Sentiment Score: 0.26197
+69. 2 Top Stocks to Buy in 2023 and Hold Forever - 2023-01-18: These companies' stocks have given investors stellar growth over the last five years, even after a sell-off in 2022., Author: Dani Cook, Source: Motley Fool, Sentiment Score: 0.261406
+70. Futures Rise Ahead Of Wholesale Inflation Report; Tesla Extends Gains - 2023-01-18: Dow Jones Futures Rise Ahead Of Key Inflation Report. Tesla Stock ... Investor's Business Daily ..., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.190415
+71. Apple Is Taking on Meta in Virtual Reality. It's Not Going to Be Easy. - 2023-01-18: Apple Wants to Play in the Metaverse. Don't Expect It to Be Easy. ..., Author: Adam Clark, Source: Barrons, Sentiment Score: 0.0
+72. OPEX Looms: 3 Reasons Markets May Need to Digest - 2023-01-18: Markets have been on a tear the past three weeks as inflation fears among investors have dissipated. Today, Andrew Rocco discusses why the market is showing some subtle signs that it may need to take a breather in the short term., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.0286
+73. Spotify joins media firms to urge EU action against Apple's 'unfair' practices - 2023-01-18: Spotify joins media firms to urge EU action against Apple's 'unfair ... ..., Author: Reuters, Source: Reuters, Sentiment Score: -0.151844
+74. Jim Cramer's top 10 things to watch in the market Wednesday: Inflation cools, Microsoft job cuts - 2023-01-18: Ahead of Wednesday's session, the Nasdaq kept its rally going, now at seven straight sessions., Author: Jim Cramer, Source: CNBC, Sentiment Score: 0.196936
+75. Apple Is Taking on Meta in Virtual Reality. It's Not Going to Be Easy. - 2023-01-18: Apple Wants to Play in the Metaverse. Don't Expect It to Be Easy. ..., Author: Adam Clark, Source: Barrons, Sentiment Score: 0.0
+76. Tesla Has the Most Valuable Car Brand, but It Isn't the Strongest - 2023-01-18: Tesla Has the Most Valuable Car Brand. Too Bad It Isn't the Strongest. ..., Author: Al Root, Source: Barrons, Sentiment Score: 0.26197
+77. Apple introduces the new HomePod with breakthrough sound and intelligence - 2023-01-18: Delivering incredible audio quality, enhanced Siri capabilities, and a safe and secure smart home experience Apple® today announced HomePod® ( 2nd generation ) , a powerful smart speaker that delivers next-level acoustics in a gorgeous, iconic design., Author: Unknown Author, Source: Investing News Network, Sentiment Score: 0.346785
+78. Down 22% to 30%, 3 Warren Buffett Dividend Stocks to Buy Right Now - 2023-01-18: This blend of growth and value provides a range of options for 2023 and beyond., Author: and Lee Samaha, Source: Motley Fool, Sentiment Score: 0.128204
+79. Better Buy in 2023: Apple Stock vs. Amazon Stock - 2023-01-18: These tech titans had a challenging 2022, but one company's performance under economic strain suggests it is the more reliable investment., Author: Dani Cook, Source: Motley Fool, Sentiment Score: 0.282339
+80. U.S. corporate greed has gone too far, says Norway fund manager who voted against Apple CEO's pay - 2023-01-18: U.S. corporate greed has gone too far, says a Norway fund manager who voted against Apple's executive compensation as part of a stringent ESG review., Author: Rachel Koning Beals, Source: MarketWatch, Sentiment Score: 0.028716
+81. 2 Million Bikes Are Stolen Every Year - This Startup Is Making Sure It Never Happens Again - 2023-01-18: If you regularly ride your bike, you know how often people mess with it. You can lock up your bike's frame, but someone steals the front tire. You lock up everything, but someone cuts the chain, and they're gone. It's a bike, so the cops are unlikely to do anything, and it's hard to track, so ..., Author: Caleb Naysmith, Source: Benzinga, Sentiment Score: 0.168612
+82. Apple Resurrects the Full-Size HomePod - 2023-01-18: The $299 speaker has room-sensing technology and sensors that listen for smoke and carbon-monoxide alarms., Author: Joseph De Avila, Source: Wall Street Journal, Sentiment Score: 0.417157
+83. Spotify Teams Up With European Companies For Regulatory Action Against Apple - 2023-01-18: Music streaming service Spotify Technology S.A. SPOT joined other media firms like Deezer to urge the European Commission to punish Apple Inc AAPL for anti-competitive and unfair practices., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: -0.326066
+84. GE Has Been One of the Best Stocks of 2023. Can It Continue? - 2023-01-18: General Electric has rallied in every session so far in 2023. Here's how we're trading this one now., Author: Bret Kenwell, Source: The Street, Sentiment Score: 0.159415
+85. Roblox's  ( RBLX )  December Metrics Indicate Promising Growth - 2023-01-18: Roblox (RBLX) sees increased engagement as estimated bookings and daily active users show growth for December., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.280221
+86. Apple HomePod  ( 2nd Gen ) : Pricing, Features, and Preorders - 2023-01-18: Apple's second-generation HomePod boasts improved audio and new smart home features., Author: Jacob Krol, Source: The Street, Sentiment Score: 0.311187
+87. Here Come the FAANG Earnings Charts - 2023-01-18: The market's "sure things" fell from grace in 2022. Will 2023 be the year for a rebound?, Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.012211
+88. Google Reportedly Working on Apple AirTag Alternative As Personal Tracker Market Sees Growth and Consolidation - 2023-01-18: Apple Inc.'s AAPL AirTags have remained dominant in the Bluetooth tracker market, with people spending billions to help keep track of their things. But there hasn't been a viable alternative., Author: Caleb Naysmith, Source: Benzinga, Sentiment Score: 0.187945
+89. Sharply Lower PPI, Retail Sales Data Further Signs of a Slowing Economy - 2023-01-18: ( Wednesday Market Open ) Just checking. Is bad economic news still good for the markets? Investors might be asking themselves that this morning as major stock indexes climbed just slightly in premarket trading despite a batch of inflation and retail sales data suggesting a slowing economy., Author: TD Ameritrade Network, Source: Benzinga, Sentiment Score: -0.014419
+90. Microsoft Is Laying Off Thousands. Here's What It Means for Investors. - 2023-01-18: The company says it is cutting 10,000 jobs., Author: Jeremy Bowman, Source: Motley Fool, Sentiment Score: 0.021651
+91. Dow Jones Falls Despite Cooling Inflation Signs; Tesla Falls As Trial Begins On Musk's 2018 Tweet - 2023-01-18: Dow Jones Falls Despite Cooling Inflation Signs. Tesla Falls As Trial ... Investor's Business Daily ..., Author: VIDYA RAMAKRISHNAN, Source: Investors Business Daily, Sentiment Score: -0.007372
+92. Apple Could Boost Profits by Designing Its Own iPhone Parts, Analyst Says - 2023-01-18: Apple could get a substantial earnings boost if the company moves ahead on plans to bring production of additional iPhone components in-house, Evercore ISI analyst Amit Daryanani asserts in a research note Wednesday., Author: Eric J. Savitz, Source: Barrons, Sentiment Score: 0.144866
+93. Alphabet  ( GOOGL )  to Expand Portfolio With Grogu Tracker - 2023-01-18: Alphabet (GOOGL) is developing a new tracking device which includes Bluetooth and ultra-wideband connectivity to help Pixel phone users to connect with compatible devices., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.348943
+94. Dow Reverses Lower On Hawkish Fed, Weak Economic Data - 2023-01-18: Dow Jones Reverses Lower On Fed, Recession Fears. Tesla ... Investor's Business Daily ..., Author: ED CARSON, Source: Investors Business Daily, Sentiment Score: -0.031876
+95. Why Qualcomm Stock Defied Gravity Today - 2023-01-18: News of a fresh dividend payment trumped an analyst's negative move on the company's shares., Author: Eric Volkman, Source: Motley Fool, Sentiment Score: 0.082955
+96. Apple HomePod Second-Gen: First Listen, Hands-On - 2023-01-18: Yes, Apple's full-sized smart speaker is back and we've listened to it., Author: Jacob Krol, Source: The Street, Sentiment Score: 0.333293
+97. Can Tech Stocks Realistically Help You Retire Early? - 2023-01-19: Retiring early with tech stocks may depend on embracing a counterintuitive investment principle., Author: Jon Quast, Source: Motley Fool, Sentiment Score: 0.150348
+98. 2 Warren Buffett ETFs to Stock Up On in 2023 - 2023-01-19: These investments could help you make a lot of money., Author: Katie Brockman, Source: Motley Fool, Sentiment Score: 0.109865
+99. Up 133% Already in 2023, Is This Metaverse Crypto a Buy? - 2023-01-19: The metaverse is now one of the hottest segments of the crypto market, and Decentraland is leading the way., Author: Dominic Basulto, Source: Motley Fool, Sentiment Score: 0.031359
+100. Better Buy: Apple Stock vs. Disney Stock - 2023-01-19: These companies are both titans of their industries, but one offers far more bang for your buck., Author: Dani Cook, Source: Motley Fool, Sentiment Score: 0.312065
+101. Should WisdomTree U.S. LargeCap Dividend ETF  ( DLN )  Be on Your Investing Radar? - 2023-01-19: Style Box ETF report for ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.228642
+102. Futures fall as weak data fuel recession worries, Fed comments on tap - 2023-01-19: Jan 19 ( Reuters ) - U.S. stock index futures fell on Thursday after weak economic data fueled recession worries, while investors await comments from more Federal Reserve officials for clues on the central bank's path of monetary tightening., Author: Reuters, Source: Reuters, Sentiment Score: -0.228341
+103. Apple Investors Have Reason To Cheer As iPhone's Share Of Global Smartphone Market Climbs To Record In Q4 - 2023-01-19: Apple Inc. AAPL is scheduled to report its fiscal year 2023, first-quarter results on Feb. 2 and investors are fretting over the impact China production disruptions and the economic softness may have had on the quarter's performance., Author: Shanthi Rexaline, Source: Benzinga, Sentiment Score: 0.13566
+104. India flexes its muscle at Davos as China's star fades | Business - 2023-01-19: India flexes its muscle at Davos as China's star fades CNN International ..., Author: Julia Horowitz, Source: CNN, Sentiment Score: 0.095442
+105. India flexes its muscle at Davos as China's star fades | Business - 2023-01-19: India flexes its muscle at Davos as China's star fades CNN International</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Predicted Stock Closing Prices for Next 12 Weeks (Fridays):
+2023-01-27: 144.9385, 2023-02-03: 153.4503, 2023-02-10: 150.2124, 2023-02-17: 151.7443, 2023-02-24: 145.9351, 2023-03-03: 150.2323, 2023-03-10: 147.7157, 2023-03-17: 154.1814, 2023-03-24: 159.4036, 2023-03-31: 164.0291, 2023-04-14: 164.3374, 
+Predicted Market Sentiment: 0.1447795348837209</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-01-13</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Week Ending on 2023-01-13:
+News Summary:
+1. Apple begins hiring retail store employees in India: Report - 2023-01-09: The company's careers page lists several different opportunities for workers in India, including business expert, "genius," operations expert and technical specialist., Author: Unknown Author, Source: Money Control, Sentiment Score: 0.125298
+2. Will iPhone Have A Challenger? OnePlus Co-Founder Says New Smartphone Will Take On Apple In US - Apple  ( NASDAQ:AAPL )  - 2023-01-09: Carl Pei, the co-founder of OnePlus, is planning to take on Apple Inc. AAPL in the U.S. by bringing a new Nothing smartphone to the market. What Happened: Nothing, a U.K.-based consumer tech startup, is in early conversations with U.S. carriers about launching a new smartphone in the country, ..., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.180745
+3. Apple Has Canceled The Next iPhone SE, Top Analyst Says - Apple  ( NASDAQ:AAPL )  - 2023-01-09: Apple Inc. AAPL has instructed suppliers about canceling the 2024 iPhone SE 4, according to a top analyst of the Cupertino-based tech giant., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: 0.037868
+4. Applied Materials Gained 7% in the Second Half of 2022. Is the Worst Over? - 2023-01-09: The semiconductor equipment company should benefit from a reshuffling of the computer chip supply chain this decade., Author: Brett Schafer, Source: Motley Fool, Sentiment Score: 0.093032
+5. iPhone exports double to surpass $2.5 billion this fiscal - 2023-01-09: India is emerging as Apple Inc.'s next manufacturing hub as assembly partners seek to add resilience to a supply chain heavily centered on China and shaken by its geopolitical and health challenges., Author: Unknown Author, Source: Money Control, Sentiment Score: 0.083826
+6. 2 Warren Buffett Stocks That Are No-Brainer Buys and 1 to Avoid Like the Plague - 2023-01-09: Two Buffett stocks stand out as clear-cut buys in the new year, while another top holding has lost much of its luster., Author: Sean Williams, Source: Motley Fool, Sentiment Score: 0.112946
+7. Apple Watch User Says He Ended Up In Emergency Room After His Gadget Exploded - Apple  ( NASDAQ:AAPL )  - 2023-01-09: An Apple Inc. AAPL watch user reportedly ended up in an emergency room after his device expanded, overheated, started smoking and eventually exploded, all in the course of an evening and night, in October 2022., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: -0.148184
+8. Grid Computing Market Is Expected to Hit USD 10,785 Million at a CAGR of 16.14% by 2030 - Report by Market Research Future  ( MRFR )  - 2023-01-09: New York, US, Jan. 09, 2023 ( GLOBE NEWSWIRE ) -- According to a comprehensive research report by Market Research Future ( MRFR ) , "Grid Computing Market Research Report, By Components, Graphics Type, by End User, by Application- Forecast till 2030, the market is anticipated to acquire a ..., Author: Globe Newswire, Source: Benzinga, Sentiment Score: 0.269343
+9. Should Invesco Dynamic Large Cap Growth ETF  ( PWB )  Be on Your Investing Radar? - 2023-01-09: Style Box ETF report for ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.30836
+10. Ahead Of Tech Earnings, Analyst Says Sector Is 'Under-Owned' - Repeats Calls For 20% Rally - SPDR Select Sector Fund - Technology  ( ARCA:XLK )  - 2023-01-09: Tech earnings news flow will hit Wall Street in earnest in two weeks and an analyst at Wedbush painted a positive picture concerning the prospects for the sector. Guidance The Key: As the focus shifts to fourth-quarter earnings, the wildcard would be the 2023 guidance and overall demand ..., Author: Shanthi Rexaline, Source: Benzinga, Sentiment Score: 0.073967
+11. Apple's India-Made iPhone Exports Surpass $2.5B In 9 Months - Nearly Twice Previous Fiscal Year's Total - Apple  ( NASDAQ:AAPL ) , Hon Hai Precision  ( OTC:HNHPF ) , Wistron  ( OTC:WICOF ) , Pegatron  ( OTC:PGTRF )  - 2023-01-09: Apple Inc. AAPL exported more than $2.5 billion worth of iPhones from India between April and December as the company diversified production amid supply disruptions in China., Author: Navdeep Yadav, Source: Benzinga, Sentiment Score: -0.04005
+12. Apple's India Hirings Signal Flagship Store Debut By March: FT - Apple  ( NASDAQ:AAPL )  - 2023-01-09: Apple Inc AAPL started hiring retail store workers in India with room for more as it eyed its flagship location debut in the promising smartphone market by this quarter., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: 0.176713
+13. Jack Ma Ceding Control In Ant, Brazil's 'Capitol Hill Moment,' Goldman Sachs Job Cut Rumors And More: 5 Key Stories You May Have Missed From The Weekend - Apple  ( NASDAQ:AAPL )  - 2023-01-09: The lull that characterized the holiday period continued into the past weekend. News flow is likely to pick up pace after the Martin Luther King Jr. holiday scheduled for Jan. 16, as the curtains lift on the fourth-quarter reporting season. Here's a recap of a few major headlines that hit the ..., Author: Shanthi Rexaline, Source: Benzinga, Sentiment Score: -0.074838
+14. Solana Dropped 90% Last Year, But Has Kicked Off 2023 With a Bang. Is This Bull Rally Real? - 2023-01-09: The Bonk crypto is restoring a sense of optimism to Solana at a time when it needed it most., Author: Michael Byrne, Source: Motley Fool, Sentiment Score: 0.053275
+15. Futures Rise Ahead Of Q4 Earnings Season - 2023-01-09: Dow Jones futures came off early highs Monday, wrestling to add to Friday's powerful stock market gains. Fourth-quarter earnings season kicks off this week, with highly anticipated results from Dow Jones members JPMorgan Chase ( JPM ) and UnitedHealth Group ( UNH ) ., Author: SCOTT LEHTONEN, Source: Investors Business Daily, Sentiment Score: 0.224053
+16. Top 5 Momentum Stocks for January After a Disappointing 2022 - 2023-01-09: We have narrowed our search on five momentum stocks with strong potential in 2023. These are: DOCU, ANET, CAG, PCTY and SCCO., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.252018
+17. Top Stories Monday, Jan. 09 - Apple  ( NASDAQ:AAPL ) , AstraZeneca  ( NASDAQ:AZN )  - 2023-01-09: Apple Inc AAPL exported more than $2.5 billion worth of iPhones from India between April and December as the company diversified production amid supply disruptions in China. The total export of the Cupertino-based tech giant in the first nine months of the fiscal year ending March 2023 was almost ..., Author: Vandana Singh, Source: Benzinga, Sentiment Score: 0.115554
+18. Apple  ( AAPL )  Expands Fitness+ With New Kickboxing Workout - 2023-01-09: Apple (AAPL) is expanding its Fitness+ content with the introduction of Kickboxing, a new meditation theme, Sleep and Beyonce to Artist Spotlight., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.148564
+19. This Day In Market History, Jan. 9: Apple Introduces The iPhone  ( NASDAQ:AAPL )  - Apple  ( NASDAQ:AAPL )  - 2023-01-09: Each day, Benzinga takes a look back at a notable market-related moment that happened on this date. On this day in 2007, Apple Inc. AAPL unveiled the first iPhone after two and a half years of hushed development. The S&amp;P 500 closed at 1,412.11, while the Dow Jones Industrial Average closed at ..., Author: Elizabeth Balboa, Source: Benzinga, Sentiment Score: 0.165969
+20. Stock Market Gains As Earnings Season Begins; Retail Stocks Sag On Weak Lululemon, Macy's Forecasts - 2023-01-09: Stock Market Gains As Earnings Season Begins. Retail Stocks Sag ... Investor's Business Daily ..., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.138051
+21. 2 Stocks to Watch From the Challenging Computer Industry - 2023-01-09: The Computer - Mini Computers industry is suffering from massive supply-chain and logistical issues, as well as geopolitical challenges. However, the strong demand for laptops and tablets bodes well for Apple (AAPL) and Lenovo (LNVGY)., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.212626
+22. Why Apple Was Rising Today - 2023-01-09: On a good day for tech stocks, Bloomberg hinted that Apple's new AR/VR headset will be released in the next couple of months., Author: Billy Duberstein, Source: Motley Fool, Sentiment Score: 0.098048
+23. Warren Buffett's Berkshire Hathaway Stock Is Breaking Out - 2023-01-09: Berkshire Hathaway stock is trying for a big-time breakout. Here's the setup., Author: Bret Kenwell, Source: The Street, Sentiment Score: 0.267281
+24. The iPhone Was Unveiled 16 Years Ago, Here's How Much $1,000 Invested In Apple Stock After The Debut Is Worth Today - Apple  ( NASDAQ:AAPL )  - 2023-01-09: Many people around the world recognize the iPhone from Apple Inc AAPL as one of the leading smartphones today. The revolutionary phone was unveiled 16 years ago by Apple co-founder and former CEO Steve Jobs. Here's a look at the announcement and how the stock performed since its debut., Author: Chris Katje, Source: Benzinga, Sentiment Score: 0.23066
+25. Short Sellers Profited By 31% in 2022 on Stock Picks - 2023-01-09: Tesla was the number one stock that short sellers made money from in 2022., Author: Ellen Chang, Source: The Street, Sentiment Score: 0.271605
+26. Look for a big cut to TSMC's 2023 outlook as a bullish sign for chips, one analyst says ahead of earnings - 2023-01-09: The best thing TSMC can do in its earnings report Thursday is to cut its outlook for 2023 big ..., Author: Wallace Witkowski, Source: MarketWatch, Sentiment Score: 0.094352
+27. Shopify Is Innovating Across All Stripes In an Effort To Slash Costs - Shopify  ( NYSE:SHOP ) , Apple  ( NASDAQ:AAPL ) , Amazon.com  ( NASDAQ:AMZN )  - 2023-01-09: Rising inflation and higher interest rates are weakening consumers' buying power and consequently, e-commerce purchases are dropping., Author: Upwallstreet, Source: Benzinga, Sentiment Score: 0.10611
+28. Samsung Is First to Succumb to a Slowing Economy That Is Crushing Semiconductors - Apple  ( NASDAQ:AAPL ) , Amazon.com  ( NASDAQ:AMZN )  - 2023-01-09: On Friday, Samsung Electronics Co. Ltd ( KSE: 005930.KS ) flagged its October-December operating quarterly profit has tumbled by two-thirds to an eight-year low as a sluggish global economy hammered memory chip prices and weakened demand for electronic devices., Author: Upwallstreet, Source: Benzinga, Sentiment Score: -0.166321
+29. Apple's iPad Mini Is $100 Off On Amazon - 2023-01-09: The most compact iPad is back to the lowest price ever on Amazon., Author: Jacob Krol, Source: The Street, Sentiment Score: 0.259649
+30. Sen. Mark Warner: 'Let's restart antitrust' tech legislation - 2023-01-09: Senator admits he's "frustrated" by the continued absence of major antitrust tech law, says kids safety protections online could be a bipartisan building block this year for a "breakthrough." ..., Author: Jon Swartz, Source: MarketWatch, Sentiment Score: 0.024373
+31. Disney CEO Bob Iger wants employees to return to the office four days a week - 2023-01-09: "Starting March 1, employees currently working in a hybrid fashion will be asked to spend four days a week on-site, targeting Monday through Thursday as in-person workdays," Iger said in an internal email obtained by MarketWatch., Author: Jon Swartz, Source: MarketWatch, Sentiment Score: 0.114442
+32. Exclusive: Top 10 Most Searched Tickers On Pro In 2022 - Where Do SPY, Tesla, Apple And AMC Rank? - SPDR S&amp;P 500  ( ARCA:SPY )  - 2023-01-09: Each trading day features hundreds of headlines and press releases on Benzinga Pro, a leading source for traders to see the latest news on the overall market and individual tickers all in one convenient location. Here is a look at the most-searched stocks on Benzinga Pro for 2022, ranked in order., Author: Chris Katje, Source: Benzinga, Sentiment Score: 0.102382
+33. Broadcom stock dinged in final minutes on report Apple working on its own WiFi/Bluetooth chips - 2023-01-09: Broadcom shares closed sharply lower Monday in the final minutes of trading following a report that Apple was working on its own WiFi and Bluetooth chips., Author: Wallace Witkowski, Source: MarketWatch, Sentiment Score: -0.100267
+34. Futures: Rally Stumbles Ahead Of Powell Speech - 2023-01-09: Dow Jones Reverses Lower Ahead Of Powell Speech. 7 Best Stocks ... Investor's Business Daily ..., Author: SCOTT LEHTONEN, Source: Investors Business Daily, Sentiment Score: 0.200029
+35. Why Microsoft Stock Topped the Market Today - 2023-01-09: Investors were cheered by a relatively small, yet meaningful, asset buy., Author: Eric Volkman, Source: Motley Fool, Sentiment Score: 0.213314
+36. S&amp;P 500 near flat as investors weigh chances of less aggressive rate hikes - 2023-01-10: The Dow ended lower, and the Nasdaq Composite ( .IXIC ) ended well off the day's highs., Author: Unknown Author, Source: Money Control, Sentiment Score: -0.048218
+37. Why Qualcomm Stock Got Mashed on Monday - 2023-01-10: A major business partnership will apparently fade away sooner rather than later., Author: Eric Volkman, Source: Motley Fool, Sentiment Score: 0.08299
+38. Apple retail stores to be spread over 25,000 sq ft in Delhi, Mumbai | The Financial Express - 2023-01-10: Apple retail stores to be spread over 25,000 sq ft in Delhi, Mumbai The Financial Express ..., Author: Unknown Author, Source: The Financial Express, Sentiment Score: 0.236502
+39. Tesla, Apple, Nuwellis, Revance, Lululemon: Why These 5 Stocks Are Drawing Investors' Attention Today - Lululemon Athletica  ( NASDAQ:LULU ) , Nuwellis  ( NASDAQ:NUWE ) , Apple  ( NASDAQ:AAPL ) , Broadcom  ( NASDAQ:AVGO ) , Tesla  ( NASDAQ:TSLA ) , Revance Therapeutics  ( NASDAQ:RVNC )  - 2023-01-10: Major Wall Street indices closed mixed on Monday with the Nasdaq Composite being the only one to end the session on a positive note, led by gains in technology shares. The Dow Jones and the S&amp;P 500 ended in the red., Author: Bhavik Nair, Source: Benzinga, Sentiment Score: 0.182107
+40. Apple VP Of Services Peter Stern Reportedly Leaving Company - Apple  ( NASDAQ:AAPL )  - 2023-01-10: Apple Inc AAPL Vice-President of Services Peter Stern is reportedly leaving the tech giant. What Happened: Stern heads Apple's services business which envelops News+, Fitness+, and iCloud+ along with other subscription services., Author: Shivdeep Dhaliwal, Source: Benzinga, Sentiment Score: -0.04065
+41. Inari Amertron falls after report that Apple plans to drop broadcom chip - 2023-01-10: Bloomberg News reported late Monday that Apple, as part of its effort to develop its own chips, plans to stop using a Broadcom part in 2025., Author: Ying Xian Wong, Source: MarketWatch, Sentiment Score: 0.016647
+42. Epson SureLab D1070 High-Production Minilab Printer is Now Available - 2023-01-10: LOS ALAMITOS, Calif., Jan. 10, 2023 /PRNewswire/ -- Epson today announced the SureLab® D1070 Minilab Photo Printer is now available. Designed for retail, event and e-commerce applications, the drylab printer is built for high-volume photo and graphic production and engineered for reliable, ..., Author: Unknown Author, Source: Business Insider, Sentiment Score: 0.29206
+43. Apple Set To Bring Radical Transformation In Chip Industry With Plan To Ditch Broadcom, Qualcomm As Suppliers: Report - Apple  ( NASDAQ:AAPL ) , Broadcom  ( NASDAQ:AVGO ) , Qualcomm  ( NASDAQ:QCOM )  - 2023-01-10: Apple Inc. AAPL has been stepping up efforts to diversify away from chip suppliers and use its own silicon in its hardware devices. What Happened: Apple is planning to replace a key part supplied by Broadcom Inc. AVGO with an in-house component by 2025, Bloomberg reported, citing people familiar ..., Author: Shanthi Rexaline, Source: Benzinga, Sentiment Score: 0.042339
+44. The Zacks Analyst Blog Highlights Arista Networks, Conagra Brands, DocuSign, Southern Copper and Paylocity Holding - 2023-01-10: Arista Networks, Conagra Brands, DocuSign, Southern Copper and Paylocity Holding are included in this Analyst Blog., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.244951
+45. Zacks Industry Outlook Highlights Apple and Lenovo - 2023-01-10: Apple and Lenovo have been highlighted in this Industry Outlook article., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.217017
+46. Apple's Push for In-House Chips Hits Suppliers Broadcom and Qualcomm - 2023-01-10: Apple's Push for In-House Chips Hits Suppliers Broadcom and ..., Author: Adam Clark, Source: Barrons, Sentiment Score: 0.029938
+47. Better Semiconductor Stock: ASML vs. Qualcomm - 2023-01-10: Which blue-chip semiconductor stock is the better long-term investment?, Author: Leo Sun, Source: Motley Fool, Sentiment Score: -0.04753
+48. Better Buy: Tesla vs. Amazon - 2023-01-10: These two growth stocks were big market underperformers in 2022., Author: Daniel Foelber and Howard Smith, Source: Motley Fool, Sentiment Score: 0.230636
+49. Taiwan Semiconductor's December Revenue Slumps Sequentially As China's COVID Chaos &amp; Macro Headwinds Weigh - Taiwan Semiconductor  ( NYSE:TSM )  - 2023-01-10: Taiwan Semiconductor Manufacturing Company Ltd's TSM December revenue of NT$192.56 billion declined 13.5% month-over-month. The revenue grew by 23.9% Y/Y. Revenue for January through December 2022 totaled NT$2.26 trillion, up by 42.6% Y/Y., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: -0.190867
+50. Broadcom Stock Slips On Report Apple Planning To Dump WiFi, Bluetooth Chips - 2023-01-10: Apple accounts for around 20% of Broadcom's overall chip sales., Author: Martin Baccardax, Source: The Street, Sentiment Score: 0.056777
+51. US Stocks Show Tentativeness On Tuesday As Traders Wait On Word From Fed Chair Jerome Powell - Invesco QQQ Trust, Series 1  ( NASDAQ:QQQ ) , SPDR S&amp;P 500  ( ARCA:SPY )  - 2023-01-10: U.S. stocks look set to start Tuesday's session on a nervous note as traders may prefer to wait and watch the inflation data before making their next moves. What Happened: Fed officials, who made public appearances on Monday, hinted at basing the magnitude of the next fed fund rate hike on the ..., Author: Shanthi Rexaline, Source: Benzinga, Sentiment Score: 0.088476
+52. Should You Invest in the iShares U.S. Technology ETF  ( IYW ) ? - 2023-01-10: Sector ETF report for ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.158969
+53. Should You Invest in the Vanguard Information Technology ETF  ( VGT ) ? - 2023-01-10: Sector ETF report for ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.129484
+54. Apple Supplier TSMC's Q4 Revenue Growth Slows Amid Demand Softness But Comes Roughly In Line With Estimates - Taiwan Semiconductor  ( NYSE:TSM )  - 2023-01-10: Taiwan Semiconductor Manufacturing Company Limited TSM, on Tuesday, reported December quarter revenues that implied that the quarterly numbers came roughly in line with estimates. The topline growth, however, slowed both from the previous quarter and the year., Author: Shanthi Rexaline, Source: Benzinga, Sentiment Score: 0.094174
+55. Indian Conglomerate Tata Nears Deal For Majority Ownership In iPhone Plant In Country - Apple  ( NASDAQ:AAPL ) , Wistron  ( OTC:WICOF )  - 2023-01-10: Tata Group neared takeover of a major Apple Inc AAPL iPhone plant in southern India in a deal likely to give the country its first homegrown iPhone maker. The airline-to-software conglomerate discussed with the factory's owner, Taiwan's Wistron Corp WICOF, for months and aimed to complete the ..., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: 0.157116
+56. Stock Market Live: Stocks Slide On Hawkish Fed Signals, Powell Speech In Focus - 2023-01-10: Fed Chair Jerome Powell is set to address a central banking conference in Stockholm prior to the start of trading., Author: Martin Baccardax, Source: The Street, Sentiment Score: -0.075664
+57. Top Stories Tuesday, Jan. 10 - Bitcoin  ( BTC/USD ) , Ethereum  ( ETH/USD )  - 2023-01-10: Coinbase Global, Inc COIN disclosed a restructuring plan letting go of 950 employees, helping it reduce its operating expenses by 25% amid the crypto meltdown., Author: Vandana Singh, Source: Benzinga, Sentiment Score: 0.106728
+58. Bruised tech investors are hedging their bets | Business - 2023-01-10: Bruised tech investors are hedging their bets ..., Author: Nicole Goodkind, Source: CNN, Sentiment Score: 0.021866
+59. Futures Fall Ahead Of Powell Speech; Boeing Slides On Downgrade - 2023-01-10: Futures Fall Ahead Of Powell Speech. Boeing Slides On Downgrade Investor's Business Daily ..., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.214453
+60. 2 Growth Stocks Down Over 25% to Buy in 2023 - 2023-01-10: As titans of their respective industries, these growth stocks are screaming buys after a sell-off in 2022., Author: Dani Cook, Source: Motley Fool, Sentiment Score: 0.262285
+61. Apple Inc.  ( AAPL )  is Attracting Investor Attention: Here is What You Should Know - 2023-01-10: Apple (AAPL) has been one of the stocks most watched by Zacks.com users lately. So, it is worth exploring what lies ahead for the stock., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.201755
+62. Stock Market News for Jan 10, 2023 - 2023-01-10: Wall Street closed mixed on Monday after a choppy session., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.0
+63. Apple's Push for In-House Chips Hits Suppliers Broadcom and Qualcomm - 2023-01-10: Apple's Push for In-House Chips Hits Broadcom and Qualcomm Stocks ..., Author: Adam Clark, Source: Barrons, Sentiment Score: 0.029938
+64. Apple Gets Ready to Storm a Big Promising Market - 2023-01-10: iPhone maker set to open first brick-and-mortar stores in world's second-largest smartphone market., Author: Luc Olinga, Source: The Street, Sentiment Score: 0.125024
+65. Spotlight Growth Shares 3 Stocks for an Uncertain &amp; Likely-Volatile 2023 - Asure Software  ( NASDAQ:ASUR ) , Apple  ( NASDAQ:AAPL )  - 2023-01-10: With 2022 now in the rearview, investors shift their focus to 2023 and the year ahead. The economic outlook for the new year remains muddied, as Wall Street looks for clues on inflation, the Federal Reserve's rate hikes, unemployment, GDP, and more. The good news?, Author: Spotlight Growth, Source: Benzinga, Sentiment Score: 0.202356
+66. Why Is Bumble  ( BMBL )  Stock Trading Higher Today - Bumble  ( NASDAQ:BMBL )  - 2023-01-10: Keybanc analyst Justin Patterson upgraded Bumble Inc BMBL from Sector Weight to Overweight and a $27 price target. The re-rating reflected positive revisions to Patterson's EBITDA forecast., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: 0.327488
+67. Got $1,000? 5 Buffett Stocks to Buy and Hold Forever - 2023-01-10: These Buffett-backed stocks could help you crush the market., Author: Keith Noonan, Source: Motley Fool, Sentiment Score: 0.249852
+68. 6 Best Music Stocks to Buy in 2023 - 2023-01-10: If you're looking for exposure to the music industry, this list will get you started., Author: Jeremy Bowman, Source: Motley Fool, Sentiment Score: 0.21832
+69. This Top Chip Stock Is Expanding Into EVs -- Is It a Buy for 2023? - 2023-01-10: Skyworks Solutions is starting small but growing fast in the electric vehicle market., Author: Nicholas Rossolillo, Source: Motley Fool, Sentiment Score: 0.221871
+70. Apple, Microsoft And Other Information Technology Stocks From 's Most Accurate Analysts - Microsoft  ( NASDAQ:MSFT ) , Apple  ( NASDAQ:AAPL )  - 2023-01-10: Wall Street analysts make new stock picks on a daily basis. Unfortunately for investors, not all analysts have particularly impressive track records at predicting market movements. Even when it comes to one single stock, analyst ratings and price targets can vary widely, leaving investors ..., Author: Lisa Levin, Source: Benzinga, Sentiment Score: 0.035317
+71. Lots Of News, Flattish Markets - Bitcoin  ( BTC/USD ) , Apple  ( NASDAQ:AAPL )  - 2023-01-10: Coinbase COIN is doing layoffs again. 20% of its staff will be let go, just 7 months after they cut 18% of their workforce. Spoke briefly at an event hosted by Swedish central bank "We are not, and will not be, a 'climate policymaker'" CPI headline inflation set to fall to 6.4% from 7.1% in ..., Author: GRIT Capital, Source: Benzinga, Sentiment Score: -0.075555
+72. 1 Green Flag and 1 Red Flag for Apple Stock in 2023 - 2023-01-10: Apple faces near-term challenges, but investors would do well to focus on the bigger picture., Author: Harsh Chauhan, Source: Motley Fool, Sentiment Score: 0.117186
+73. Apple Chip Risk to Broadcom Isn't Material, Says Analyst - 2023-01-10: Bernstein is downplaying the potential risk to Broadcom from a recent report that says Apple is looking to replace some of the supplier's business with an in-house design., Author: Tae Kim, Source: Barrons, Sentiment Score: 0.086495
+74. Battery Maker Enovix Hopes To Recharge With New CEO, Strategy - 2023-01-10: Enovix Stock Looks To Regain Investor Confidence Investor's Business Daily ..., Author: PATRICK SEITZ, Source: Investors Business Daily, Sentiment Score: 0.146028
+75. Could Apple WiFi chips just be a ploy to get a better deal from Broadcom? - 2023-01-10: Broadcom shares fell on reports that Apple was working on its own RF chips, but one analyst wondered if it was all a negotiating ploy., Author: Wallace Witkowski, Source: MarketWatch, Sentiment Score: 0.106427
+76. Everyone's Worst Fears About the Roomba Have Come True - 2023-01-10: Read this before you buy a robot vacuum of any kind., Author: Colette Bennett, Source: The Street, Sentiment Score: 0.115426
+77. IBM just broke a winning streak that lasted nearly three decades - 2023-01-10: IBM lost its crown as the top U.S. patent grantee in 2022 to South Korea's Samsung, according to a ranking from an industry tracker ..., Author: Wallace Witkowski, Source: MarketWatch, Sentiment Score: 0.136972
+78. Mega Millions Tops $1.1 Billion: Here's How Much You'll Actually Win And 10 Things You Can Buy With The Winnings - SPDR S&amp;P 500  ( ARCA:SPY )  - 2023-01-10: If you've ever dreamed of instantly having hundreds of millions of dollars to buy whatever you want, the Mega Millions might be calling your name on Tuesday. For the fourth time in four years, the jackpot on the Mega Millions lottery drawing has topped the $1 billion mark., Author: Chris Katje, Source: Benzinga, Sentiment Score: 0.381523
+79. Market Reclaims Key Levels Ahead Of CPI Inflation Report - 2023-01-10: Dow Jones futures were little changed after hours, along with S&amp;P 500 futures and Nasdaq futures. The stock market rally was indecisive for much of Tuesday, but the major indexes gained steam, with the S&amp;P 500 moving its 50-day moving average. Investors await the December CPI inflation report on ..., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.088456
+80. Apple  ( AAPL )  Gains But Lags Market: What You Should Know - 2023-01-10: Apple (AAPL) closed the most recent trading day at $130.73, moving +0.45% from the previous trading session., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.125112
+81. The holiday PC market stunk for everyone except Apple, report says - 2023-01-11: A sharp drop in global PC shipments in the holiday quarter makes it more likely that the PC market's recovery will be later than expected., Author: Wallace Witkowski, Source: MarketWatch, Sentiment Score: -0.101726
+82. Apple Makes Move Toward Making Own iPhone, Watch Screens - Apple  ( NASDAQ:AAPL )  - 2023-01-11: Apple Inc AAPL is reportedly making a move away from mobile manufacturing partners like Samsung and LG as it plans to use its own displays in 2024. What Happened: At the beginning, Apple plans to use its own display in the highest-end Apple Watches by the end of 2024, Bloomberg reported, citing ..., Author: Shivdeep Dhaliwal, Source: Benzinga, Sentiment Score: 0.076775
+83. Apple Watch Faces Potential Import Ban As US Judge Rules Against Tech Giant In Patent Infringement Case - Apple  ( NASDAQ:AAPL ) , Masimo  ( NASDAQ:MASI )  - 2023-01-11: Apple Inc.'s AAPL smartwatches could face an import ban as a U.S. judge ruled that the company infringed on one of Masimo's MASI pulse oximeter patents., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: -0.068394
+84. Apple Supplier Plans To Invest $400M For New Vietnam Factories Amid China Tensions - Samsung Electronics Co  ( OTC:SSNLF ) , Apple  ( NASDAQ:AAPL )  - 2023-01-11: Apple Supplier Plans To Invest $400M For New Vietnam Factories Amid China Tensions Apple Inc. AAPL supplier BOE Technology Group plans to build two factories in Vietnam., Author: Navdeep Yadav, Source: Benzinga, Sentiment Score: -0.021132
+85. The 'best places to work' in America are dominated by tech companies - but these three Silicon Valley giants did not make the list - 2023-01-11: The names are drawn from the anonymous feedback of the employees who actually work at these companies., Author: Zoe Han, Source: MarketWatch, Sentiment Score: 0.293148
+86. $10,000 Invested in These Growth Stocks Could Make You a Fortune Over the Next 10 Years - 2023-01-11: Here are three exceptional growth stocks to buy for long-term investors., Author: Lee Samaha, Source: Motley Fool, Sentiment Score: 0.241513
+87. Stocks Higher, 10-Year Auction, Tesla, Apple, WWE - Five Things To Know - 2023-01-11: Stock futures higher as Powell avoids rate bet pushback. Treasury's 10-year bond auction in focus as CPI data looms. Tesla seeks permission for $775 million Texas factory expansion. Apple looking to use in-house display screens amid self-reliance push and WWE shares extends gains as Vince McMahon ..., Author: Martin Baccardax, Source: The Street, Sentiment Score: 0.086053
+88. Apple Is Moving More of Its Supply Chain In-House. Screens Could Be Next. - 2023-01-11: Apple 's apparent desire to move more of its components in-house could be a game-changer for its major suppliers, and not in a good way. It's not just chips that the tech giant wants to handle itself, screens could also be brought in-house., Author: Callum Keown, Source: Barrons, Sentiment Score: 0.051771
+89. 1 Warren Buffett ETF That Could Help You Retire a Millionaire - 2023-01-11: With a few hundred dollars per month, you could be on your way to millionaire status., Author: Katie Brockman, Source: Motley Fool, Sentiment Score: 0.09611
+90. Apple Investors Don't Need To Be Jittery About Near-Term 'Unit Disruptions' Ahead Of Q1 Earnings: Analyst Says This Metric More Important - Apple  ( NASDAQ:AAPL )  - 2023-01-11: Apple Inc.'s AAPL stock has baked in so much negativity as reflected by the 28% pullback since it hit an all-time intraday high of $182.94 in early January 2021. Despite the headwinds dragging fundamentals lower, an analyst at KeyBanc Capital Markets is optimistic about the stock., Author: Shanthi Rexaline, Source: Benzinga, Sentiment Score: 0.067826
+91. 3 Stocks to Buy Before the Bull Market - 2023-01-11: The bear market isn't going to last forever. Buying these stocks could set you up for some great long-term returns., Author: David Jagielski, Source: Motley Fool, Sentiment Score: 0.080399
+92. Should Schwab U.S. LargeCap Growth ETF  ( SCHG )  Be on Your Investing Radar? - 2023-01-11: Style Box ETF report for ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.292525
+93. 2 Must-Watch Big Tech Earnings Reports - 2023-01-11: These companies' upcoming earnings reports could give investors better insight into the economy., Author: Daniel Sparks, Source: Motley Fool, Sentiment Score: 0.060706
+94. Apple's December Quarter Mac Shipments Down 7.5% YoY Amid Steeper 28.7% Plunge In Global PC Sales: Canalys - Apple  ( NASDAQ:AAPL ) , Dell Technologies  ( NYSE:DELL )  - 2023-01-11: Ahead of Apple Inc.'s AAPL quarterly results due in early February, a report released by market research firm Canalys showed a high-single-digit decline in Mac shipments for the December quarter., Author: Shanthi Rexaline, Source: Benzinga, Sentiment Score: -0.12865
+95. Alphabet  ( GOOGL )  Boosts YouTube Music With Redesigned Library - 2023-01-11: Alphabet's (GOOGL) subsidiary Google is rolling out a redesigned Library tab to provide an enhanced experience to iOS and Android users., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.310386
+96. Alibaba To Rally Around 23%? Here Are 10 Other Analyst Forecasts For Wednesday - Apple  ( NASDAQ:AAPL ) , Boeing  ( NYSE:BA )  - 2023-01-11: Barclays boosted Delta Air Lines, Inc. DAL price target from $38 to $44. Barclays analyst Brandon Oglenski maintained an Overweight rating on the stock. Del</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Predicted Stock Closing Prices for Next 12 Weeks (Fridays):
+2023-01-20: 136.9333, 2023-01-27: 144.9385, 2023-02-03: 153.4503, 2023-02-10: 150.2124, 2023-02-17: 151.7443, 2023-02-24: 145.9351, 2023-03-03: 150.2323, 2023-03-10: 147.7157, 2023-03-17: 154.1814, 2023-03-24: 159.4036, 2023-03-31: 164.0291, 
+Predicted Market Sentiment: 0.11309127586206894</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023-01-06</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Week Ending on 2023-01-06:
+News Summary:
+1. Futures Mixed Ahead Of Jobs Data - 2023-01-05: Dow Jones Futures Fall On Strong Jobs Data. Silvergate Crashes ... Investor's Business Daily ..., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.048411
+2. Irish Watchdog Penalizes Meta By €390M For User Privacy Violation - Meta Platforms  ( NASDAQ:META )  - 2023-01-05: Ireland Data Protection Commission ( DPC ) disclosed the conclusion of two inquiries into the data processing operations of Meta Platforms Inc META regarding the delivery of its Facebook and Instagram services., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: -0.023583
+3. Gesture Recognition Market Size to Hit $51.48 Billion, Globally, by 2028 with 22.3% CAGR - Growth Report by The Insight Partners - 2023-01-05: New York, Jan. 05, 2023 ( GLOBE NEWSWIRE ) -- The Insight Partners published latest research study on "Gesture Recognition Market Size, Share, Growth, Trends and Global Forecast to 2028 - COVID-19 Impact and Global Analysis by Technology ( Touch-Based Gesture Recognition and Touchless Gesture ..., Author: Globe Newswire, Source: Benzinga, Sentiment Score: 0.224863
+4. First Apple Computer Trade Sign, Wozniak Tool Box to Be Auctioned - 2023-01-05: CHESAPEAKE CITY, Md., Jan. 5, 2023 /PRNewswire/ -- On January 27, 2023 Maryland auctioneers Alexander Historical Auctions, known internationally for their sale of historical objects, will be offering the first trade sign used by the world's largest company, Apple, Inc., at trade shows and at its ..., Author: PRNewswire, Source: Benzinga, Sentiment Score: 0.051898
+5. Apple Kicks off 2023 With new Features for Fitness+ - 2023-01-05: The digital fitness service is getting kickboxing workouts, sleep meditation, a new season of 'Time to Walk,' and a Beyoncè artist spotlight series., Author: Jacob Krol, Source: The Street, Sentiment Score: 0.290172
+6. Shopify Just Threw a Big Lifeline to Meta Platforms and Alphabet - 2023-01-05: The company's digital advertising tools bypass Apple's privacy measures., Author: Danny Vena, Source: Motley Fool, Sentiment Score: 0.161453
+7. What's Going On With Apple Stock Today? - Apple  ( NASDAQ:AAPL )  - 2023-01-05: Apple Inc AAPL shares are volatile on Thursday. Key supplier Foxconn, or Hon Hai Precision Industry Co Ltd HNHPF, turned in preliminary numbers for December showing production returned to normal last month., Author: Adam Eckert, Source: Benzinga, Sentiment Score: -0.004847
+8. The Most Anticipated Mobile Games Of 2023: 5 Titles To Keep An Eye On - Apple  ( NASDAQ:AAPL ) , Activision Blizzard  ( NASDAQ:ATVI )  - 2023-01-05: Despite being underestimated by some gamers, it's undeniable that the mobile gaming trend is growing by leaps and bounds year after year. Mobile games provide a form of light entertainment, allowing them to be played during the day and even in the middle of the daily routine., Author: Franca Quarneti, Source: Benzinga, Sentiment Score: -0.021678
+9. T-Mobile US Analysts Cheer Its Preliminary Q4 Subscriber Numbers - T-Mobile US  ( NASDAQ:TMUS )  - 2023-01-05: RBC Capital analyst Kutgun Maral maintained Outperform on T-Mobile US, Inc TMUS with a $166 price target after it shared preliminary 4Q22 subscriber results and provided some color at an investor conference., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: 0.091263
+10. Tech Layoffs Will Drive a Rebound, Analyst Says - 2023-01-05: Salesforce, Microsoft Top Picks. Layoffs "Positive" for Markets, Analyst Says. ..., Author: Karishma Vanjani, Source: Barrons, Sentiment Score: -0.18664
+11. Big Tech Needs To Take Positive Action To Avoid Falling From Glory - Microsoft  ( NASDAQ:MSFT ) , Apple  ( NASDAQ:AAPL ) , Amazon.com  ( NASDAQ:AMZN )  - 2023-01-05: The music for Big Tech stopped last year after the Federal Reserve's aggressive interest rate increases crushed demand for growth stocks. On top of this, regulators are going after the digital giants in an effort to get them to behave more responsibly and the growth of the cloud market is slowing ..., Author: Upwallstreet, Source: Benzinga, Sentiment Score: -0.041807
+12. Microsoft's AI Chatbot Could Bring 21% In Gains For Stockholders, But Analysts Are Torn Over Cloud Biz - Microsoft  ( NASDAQ:MSFT )  - 2023-01-05: Equity research firm Davidson is optimistic about the future of Microsoft MSFT. Analysts Gil Luria and William Jellison initiated coverage and are expecting the company's stock to gain over 21% in the next year, projecting a price target of $270 against a current price of $223., Author: Natan Ponieman, Source: Benzinga, Sentiment Score: 0.043227
+13. Why AppLovin  ( APP )  Shares Are Falling Today - AppLovin  ( NASDAQ:APP )  - 2023-01-05: Benchmark analyst Mark Zgutowicz initiated coverage on AppLovin Corp APP with a Sell rating and a price target of $7. The analyst turned cautious about AppLovin's near-term business fundamentals and long-term competitive positioning and expected additional meaningful estimate revisions ahead., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: -0.063084
+14. 3 Top Chip Stocks Paying Dividends - 2023-01-05: While it's been a rough past year to own chip stocks, these three have seen their earnings outlook recently drift higher. Is the tide turning?, Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.254217
+15. Apple Earnings Could Come In Higher-Than-Expected But Stock Appears Weak Heading Into The Event - Apple  ( NASDAQ:AAPL )  - 2023-01-05: Apple Inc AAPL was trading mostly flat on Thursday afternoon, holding more steady than the S&amp;P 500, which was declining about 1.1%. Foxconn, or Hon Hai Precision Industry Co Ltd HNHPF, a key Apple supplier, announced production numbers for the month of December that came in above previously ..., Author: Melanie Schaffer, Source: Benzinga, Sentiment Score: 0.04157
+16. Qualcomm jumps into emergency services with Snapdragon Satellite, in cooperation with Iridium - 2023-01-05: Qualcomm is looking to leapfrog Apple by offering emergency satellite service using Android smartphones., Author: Wallace Witkowski, Source: MarketWatch, Sentiment Score: -0.021481
+17. Qualcomm Launching Snapdragon Satellite: What Investors Should Know About New Product - Qualcomm  ( NASDAQ:QCOM )  - 2023-01-05: Leading technology company Qualcomm Inc QCOM announced the launch of a new product at CES 2023 Thursday. Here are the details on Snapdragon Satellite. What Happened: Qualcomm has shown off several new products and partnerships at CES 2023, held this week in Las Vegas., Author: Chris Katje, Source: Benzinga, Sentiment Score: 0.232864
+18. Looking for clues about iPhone supply? Ask AT&amp;T, Verizon and T-Mobile - 2023-01-05: How have iPhone sales have fared in the wake of production constraints on high-end models? Some public companies may have just offered a few clues., Author: Emily Bary, Source: MarketWatch, Sentiment Score: 0.037606
+19. Samsung forecasts big slump in fourth-quarter profit as tech demand wanes - 2023-01-06: The South Korean tech giant on Friday forecast its operating profit in the quarter ending Dec. 31 to drop by 69% from the prior year to 4.3 trillion won, the rough equivalent of $3.4 billion., Author: Jiyoung Sohn, Source: MarketWatch, Sentiment Score: 0.201233
+20. Samsung profit slumps by most in decade on weak demand for memory chips - 2023-01-06: Profit slumped last quarter by the most in more than a decade as memory chip prices crashed. Samsung may have to rein in capital expenditure to conserve cash, Citigroup says., Author: Bloomberg, Source: South China Morning Post, Sentiment Score: -0.244786
+21. Samsung estimates quarterly profit sank to 8-year low on demand slump | Business - 2023-01-06: Samsung estimates quarterly profit sank to 8-year low on demand slump ..., Author: Reuters, Source: CNN, Sentiment Score: 0.056317
+22. Apple's Iconic 1970s Trade Sign, Steve Wozniak's Tool Box Up For Auction - Here Are The Hefty Starting Bids - Apple  ( NASDAQ:AAPL )  - 2023-01-06: Apple Inc.'s AAPL first trade sign with a multi-colored logo and a battered toolbox used by co-founder Steve Wozniak is now up for auction - and you can get both items, but it's going to be an expensive affair., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: -0.011742
+23. Apple's Mixed Reality Headset 'Behind Schedule,' Says Analyst - January Launch 'Unlikely' - Apple  ( NASDAQ:AAPL )  - 2023-01-06: The delay in the development of Apple Inc.'s AAPL highly-anticipated mixed reality headset could hamper the company's plans to hold a media event for the device in January., Author: Ananya Gairola, Source: Benzinga, Sentiment Score: -0.049169
+24. My Top Stock to Buy for 2023  ( and It's Not Even Close )  - 2023-01-06: Amazon is the complete package at a good value., Author: Daniel Foelber, Source: Motley Fool, Sentiment Score: 0.130013
+25. 5 Stocks Warren Buffett Is Betting Big on for 2023 - 2023-01-06: The Oracle of Omaha expects five companies to outperform in the new year., Author: Sean Williams, Source: Motley Fool, Sentiment Score: 0.198412
+26. Samsung Blames Weak Demand for Profit Drop. What This Means for Apple. - 2023-01-06: Samsung Warns of Profit Drop Blaming Weak Demand. What This Means for Apple. ..., Author: Brian Swint, Source: Barrons, Sentiment Score: -0.152532
+27. Iridium, Qualcomm Join Forces To Tap Satellite Messaging Beyond Smartphones - Iridium Comms  ( NASDAQ:IRDM ) , Qualcomm  ( NASDAQ:QCOM )  - 2023-01-06: Iridium Communications Inc IRDM collaborated with Qualcomm Inc QCOM Qualcomm Technologies, Inc to enable satellite messaging and emergency services in smartphones powered by Snapdragon Mobile Platforms. Iridium satellite constellation supports Qualcomm Technologies' new Snapdragon Satellite ..., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: 0.191597
+28. You Could've Become a Millionaire With Just $1,000 Invested in This Warren Buffett Stock - 2023-01-06: If you've ever wondered about the benefits of long-term investing, this story is for you., Author: Anthony Di Pizio, Source: Motley Fool, Sentiment Score: 0.205361
+29. Should BNY Mellon US Large Cap Core Equity ETF  ( BKLC )  Be on Your Investing Radar? - 2023-01-06: Style Box ETF report for ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.170581
+30. Is Schwab Fundamental U.S. Broad Market Index ETF  ( FNDB )  a Strong ETF Right Now? - 2023-01-06: Smart Beta ETF report for ..., Author: Zacks Investment Research, Source: Zacks Commentary, Sentiment Score: 0.274062
+31. Insights on the SVOD  ( Subscription Video on Demand )  European Market to 2026 - Featuring Prime Video, Apple, Netflix and DAZN Among Others - 2023-01-06: DUBLIN, Jan. 6, 2023 /PRNewswire/ -- The "Europe SVOD ( Subscription Video on Demand ) Market: Insights &amp; Forecast with Potential Impact of COVID-19 ( 2022-2026 ) " report has been added to ResearchAndMarkets.com's offering., Author: PRNewswire, Source: Benzinga, Sentiment Score: 0.324652
+32. Are Growth Stocks in for More Pain in 2023? - 2023-01-06: Now is the time to consider buying Microsoft, Apple, Alphabet, or Amazon., Author: Daniel Foelber, Source: Motley Fool, Sentiment Score: 0.273921
+33. 4 Artificial Intelligence Stocks to Buy in 2023 - 2023-01-06: Artificial intelligence will be a big theme for the market this year and these companies are leading the way., Author: Travis Hoium, Source: Motley Fool, Sentiment Score: 0.272617
+34. Wearable Pregnancy Devices Market will worth USD 10593.96 million by 2030 : GreyViews - 2023-01-06: Pune India, Jan. 06, 2023 ( GLOBE NEWSWIRE ) -- The market has been studied for the below mentioned-segmentation and regional analysis for North America, Europe, Asia, South America, and the Middle East and Africa., Author: Globe Newswire, Source: Benzinga, Sentiment Score: 0.179389
+35. Best Mutual Funds Report: Bulls In Hibernation In Bear Market - 2023-01-06: The first list of new buys by the best mutual funds in the new year reflects the lack of a Santa Claus rally in 2022. At least for now, it's the bulls, rather than the bears, that have gone into hibernation. The dollar amounts invested by top funds into the individual stocks on this screen ..., Author: MATTHEW GALGANI, Source: Investors Business Daily, Sentiment Score: 0.170039
+36. Samsung Sees Q4 Profit Plunge 69% As Pandemic Correction And Macro Headwinds Weigh - Samsung Electronics Co  ( OTC:SSNLF )  - 2023-01-06: Samsung Electronics Co, Ltd SSNLF shared the guidance for its fourth quarter. The ace chipmaker expects consolidated sales of approximately 70 trillion Korean won, down 8.6% year-on-year. Samsung saw a consolidated operating profit of approximately 4.3 trillion Korean won., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: 0.071526
+37. Futures Higher After Strong December Jobs Report - 2023-01-06: Dow Jones Futures Rally On December Jobs Report. Tesla Stock ... Investor's Business Daily ..., Author: SCOTT LEHTONEN, Source: Investors Business Daily, Sentiment Score: 0.098496
+38. Tech Sell-Off: 2 Growth Stocks to Buy in 2023 - 2023-01-06: Apple and Nvidia suffered in 2022, but a new year brings new opportunities., Author: Dani Cook, Source: Motley Fool, Sentiment Score: 0.187058
+39. Iridium, Qualcomm To Partner In Satellite-Based Smartphone Text Services - 2023-01-06: Iridium, Qualcomm To Partner In Satellite-Based Smartphone Text ... Investor's Business Daily ..., Author: REINHARDT KRAUSE, Source: Investors Business Daily, Sentiment Score: 0.146183
+40. Apple Unusual Options Activity For January 06 - Apple  ( NASDAQ:AAPL )  - 2023-01-06: A whale with a lot of money to spend has taken a noticeably bearish stance on Apple. Looking at options history for Apple AAPL we detected 38 strange trades. If we consider the specifics of each trade, it is accurate to state that 47% of the investors opened trades with bullish expectations and ..., Author: Benzinga Insights, Source: Benzinga, Sentiment Score: 0.092361
+41. Wall St jumps as December jobs report eases rate worries | The Financial Express - 2023-01-06: Wall St jumps as December jobs report eases rate worries The Financial Express ..., Author: Unknown Author, Source: The Financial Express, Sentiment Score: -0.002421
+42. Stocks Mostly Higher; Tesla, GE In Focus: Weekly Review - 2023-01-06: Stocks Mostly Higher. Tesla, GE In Focus: Weekly Review Investor's Business Daily ..., Author: IBD STAFF, Source: Investors Business Daily, Sentiment Score: -0.159356
+43. Qualcomm Satellite Messaging Partnership Likely To Trigger Iridium's Revenue Stream, Analyst Says - Iridium Comms  ( NASDAQ:IRDM ) , Qualcomm  ( NASDAQ:QCOM )  - 2023-01-06: Qualcomm Inc QCOM has been the previously unnamed partner in Iridium Communications Inc's IRDM smartphone Technology Development Agreement and Service Provider Agreement. Snapdragon Satellite will be a satellite-based, two-way capable messaging solution for next-generation premium Android ..., Author: Anusuya Lahiri, Source: Benzinga, Sentiment Score: 0.15856
+44. Global Digital Gift Card Market Report 2022 to 2031 - Featuring Apple, Blackhawk Network Holdings, Fiserv and InComm Payments Among Others - 2023-01-06: Global Digital Gift Card Market Report 2022 to 2031 - Featuring ... PR ..., Author: Research and Markets, Source: PR Newswire, Sentiment Score: 0.357569
+45. SQ: Does Block Stock Deserve a Spot in Your Portfolio in 2023? - 2023-01-06: Block ( SQ ) is a technology company that creates tools to enable businesses, sellers, and individuals to participate in the digital economy. The company operates through two segments: Square and Cash App. Despite losing 54.9% over the past year, the stock is currently trading above its ..., Author: Unknown Author, Source: Stocknews.com, Sentiment Score: 0.012065
+46. No one's having fun in the stock market these days, and that might be a sign that a bottom is near - 2023-01-06: When apathy sets in, it will be time to begin buying tech stocks again., Author: Cody Willard, Source: MarketWatch, Sentiment Score: 0.062816
+47. Dow Jones Rallies On This; Tesla Stock Fights Back, Elon Musk Jokes; WWE Stock 'Gorilla Presses' Higher - 2023-01-06: Dow Jones Rallies On This. Tesla Stock Fights Back, Elon Musk ... Investor's Business Daily ..., Author: Investor's Business Daily, Source: Investors Business Daily, Sentiment Score: 0.265002
+48. CES 2023: AMD, Nvidia, auto applications get the hype, but analysts say this one chip maker ruled - 2023-01-06: As CES 2023 draws to a close this weekend much of the attention in the chip world was lauded on companies like Advanced Micro Devices Inc. and Nvidia Corp. but a lower profile chip maker appears better positioned coming out of the convention., Author: Wallace Witkowski, Source: MarketWatch, Sentiment Score: 0.050211
+49. Top 6 Electric Vehicle  ( EV )  ETFs in 2023 - 2023-01-06: These ETFs allow investors to bet on EVs without picking individual stocks., Author: Matthew DiLallo, Source: Motley Fool, Sentiment Score: 0.190829
+50. Verizon shares log best six-day stretch since 2020 - 2023-01-06: The new year is bringing new momentum for Verizon Communications Inc.'s stock., Author: Emily Bary, Source: MarketWatch, Sentiment Score: 0.228846
+51. 1 Warren Buffett Stock Down 27% to Buy in 2023 - 2023-01-06: Apple stock tumbled in 2022, but that has only made it more attractive., Author: Dani Cook, Source: Motley Fool, Sentiment Score: 0.366179
+52. 3 Top Tech Stocks to Buy in January - 2023-01-06: Down between 59% and 80%, these growth stocks are great buys this month., Author: Keith Noonan, Source: Motley Fool, Sentiment Score: 0.364817
+53. How to Invest in Tech ETFs - 2023-01-06: Here's how to get tech exposure without the single-stock risk., Author: Matthew Frankel, Source: Motley Fool, Sentiment Score: 0.132667
+54. FTC's proposed ban on noncompete agreements could have biggest impact on tech industry - 2023-01-06: A proposed FTC ban on noncompete agreements would apply across all industries and income levels, but could have the biggest impact on the tech industry., Author: Levi Sumagaysay, Source: MarketWatch, Sentiment Score: 0.036423
+55. Why Apple Stock Was the Apple of Investors' Eyes Today - 2023-01-06: Bargain hunters and optimistic analysts brought the bulls back at the end of the week., Author: Eric Volkman, Source: Motley Fool, Sentiment Score: 0.246836
+56. Taiwan exports fall for 4th month in December, decline seen extending into Q1 - 2023-01-07: Taiwan exports fall for 4th month in December, decline seen ... ..., Author: Reuters, Source: Reuters, Sentiment Score: -0.18391
+57. Better Buy: Tesla vs. Apple - 2023-01-07: These once red-hot stocks are now hovering around their 52-week lows., Author: Daniel Foelber and Howard Smith, Source: Motley Fool, Sentiment Score: 0.167229
+58. 3 Compelling Reasons Why Amazon Stock Is a Smarter Pick Than Apple in 2023 - 2023-01-07: Both of these stocks should remain winners over the long run. But Amazon has some near-term advantages., Author: Keith Speights, Source: Motley Fool, Sentiment Score: 0.190257
+59. 1 Unstoppable Vanguard ETF I'm Stocking Up on in 2023 - 2023-01-07: This ETF could have a lot of potential in 2023 and beyond., Author: Katie Brockman, Source: Motley Fool, Sentiment Score: 0.201854
+60. You're Thinking About Going to the Gym, but Are You Thinking About Investing in It? - 2023-01-07: And we chat about new questions to ask about growth stocks., Author: Asit Sharma, Source: Motley Fool, Sentiment Score: 0.203485
+61. Qualcomm Stock: Bear vs. Bull - 2023-01-07: The mobile chipmaker could be a divisive investment in 2023., Author: Leo Sun, Source: Motley Fool, Sentiment Score: 0.040533
+62. 3 Apple Stock Predictions for 2023 - 2023-01-07: Even the Magic 8 Ball couldn't have predicted the events of 2022. Let's see if this year will be any different., Author: Danny Vena, Source: Motley Fool, Sentiment Score: 0.135688
+63. Everyone Is Talking About This Stock. Is It a Good Long-Term Option? - 2023-01-07: Shares were down in 2022 for this streaming business, and shareholders are rightfully thinking about what to do., Author: Neil Patel, Source: Motley Fool, Sentiment Score: 0.184111
+64. A Fresh Face-Off on the Market Cap Game Show - 2023-01-07: A market cap game with the "Rule Breaker Investing" podcast., Author: Motley Fool Staff, Source: Motley Fool, Sentiment Score: 0.157481
+65. Dozens in Congress beat stock market in 2022 despite downturn on Wall Street: analysis - 2023-01-07: More than two dozen members of Congress beat the stock market despite Wall Street suffering its worst year since 2008, according to an analysis by a popular stock-trading news site., Author: Lydia Moynihan Rich Calder, Source: MarketWatch, Sentiment Score: 0.076829
+66. EXCLUSIVE: Will Alphabet, Amazon, Apple Or Tesla See Biggest Increase In 2023? 44% Of Followers Picked This Stock - SPDR S&amp;P 500  ( ARCA:SPY )  - 2023-01-07: The stock market had a rough year in 2022 with many top indexes seeing decade lows. Many large-cap technology stocks were among the biggest losers of the year. To kick off 2023, Benzinga polled its followers to see which popular stock might have the best 2023., Author: Chris Katje, Source: Benzinga, Sentiment Score: 0.0
+67. Apple, Tesla, Netflix, Microsoft And A Critic Calls Bitcoin A 'Magnet For Idiots': Bulls And Bears Of The Week - Microsoft  ( NASDAQ:MSFT )  - 2023-01-07: Benzinga examined the prospects for many investors' favorite stocks over the last week - here's a look at some of our top stories. After showing uncertainty at the start of the week, the three major indexes finished strong on Friday., Author: Michael Cohen, Source: Benzinga, Sentiment Score: 0.077978
+68. If You Invested $1,000 In Apple Stock When Donald Trump Sold, Here's The 'YUGE' Return You Would Have Today - Apple  ( NASDAQ:AAPL )  - 2023-01-07: Former President Donald Trump is no stranger to being outspoken and sharing his opinions on a range of topics. A study showed that Trump once tweeted 5,293 times in a 12-month period, ranking first among world leaders., Author: Chris Katje, Source: Benzinga, Sentiment Score: 0.243741
+69. Apple Co-Founder Says Many Cryptocurrencies Are 'Rip-Offs' But Only One Is 'Pure Gold' - Bitcoin  ( BTC/USD )  - 2023-01-07: Apple Inc. AAPL co-founder Steve Wozniak has described Bitcoin BTC/USD as the only cryptocurrency that's "pure-gold mathematics." What Happened: Wozniak made the comments about Bitcoin in an interview with Business Insider in March 2022, adding that many cryptocurrencies are untrustworthy and ..., Author: Madhukumar Warrier, Source: Benzinga, Sentiment Score: 0.110919
+70. Cathie Wood Sees Tesla Stock Hitting $500 By 2026 Even Without Autonomous Driving &amp; Ride-Hailing Service - Tesla  ( NASDAQ:TSLA )  - 2023-01-07: Tesla, Inc. TSLA bull Cathie Wood-run Ark Invest on Friday gave a new perspective on the firm's long-term price target for the stock of the electric vehicle maker. What Happened: Ark's 2026 price target for Tesla stock would be about $500 per share, based on its EV business alone, the firm's ..., Author: Shanthi Rexaline, Source: Benzinga, Sentiment Score: 0.09962
+71. 12 Stock Market Predictions for 2023 - 2023-01-08: Here's what you can expect from the U.S. economy, the stock market, and some of the most widely held companies in the new year., Author: Sean Williams, Source: Motley Fool, Sentiment Score: -0.041978
+72. Top Wall Street analysts pick these stocks to celebrate the new year - 2023-01-08: TipRanks analyst ranking service pinpoints Wall Street's best-performing stocks, including Apple and Bumble., Author: Tipranks.com Staff, Source: CNBC, Sentiment Score: 0.358923
+73. Can Shiba Inu Reach $1 in 2023? - 2023-01-08: This meme coin is down a whopping 90% from its peak., Author: Neil Patel, Source: Motley Fool, Sentiment Score: 0.20584
+74. 2 Top Stocks in Warren Buffett's Secret Portfolio to Buy Now and Hold Forever - 2023-01-08: These industry-leading growth stocks could make patient shareholders richer in the long run., Author: Trevor Jennewine, Source: Motley Fool, Sentiment Score: 0.212346
+75. Apple To Launch MR Headset After 7 Years In Development But Focus May Have Cost Innovation In Other Products, Gurman Says - Apple  ( NASDAQ:AAPL )  - 2023-01-08: Apple, Inc.'sAAPL mixed reality headset, which has been in the works since 2017, could finally see the light of day this year., Author: Shanthi Rexaline, Source: Benzinga, Sentiment Score: 0.103426
+76. Elon Musk Predicts One of San Francisco's Problems Will Get Worse - 2023-01-08: The tech mecca faces a huge problem: a surge of empty offices., Author: Luc Olinga, Source: The Street, Sentiment Score: 0.043248
+Stock Closing Prices for Past 3 Months (Fridays):
+2022-10-14: 137.2118, 2022-10-21: 146.0267, 2022-10-28: 154.4252, 2022-11-04: 137.4398, 2022-11-11: 148.6829, 2022-11-18: 150.2621, 2022-11-25: 147.1037, 2022-12-02: 146.8057, 2022-12-09: 141.1941, 2022-12-16: 133.5961, 2022-12-23: 130.9641, 2022-12-30: 129.0472, </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Predicted Stock Closing Prices for Next 12 Weeks (Fridays):
+2023-01-13: 133.8444, 2023-01-20: 136.9333, 2023-01-27: 144.9385, 2023-02-03: 153.4503, 2023-02-10: 150.2124, 2023-02-17: 151.7443, 2023-02-24: 145.9351, 2023-03-03: 150.2323, 2023-03-10: 147.7157, 2023-03-17: 154.1814, 2023-03-24: 159.4036, 2023-03-31: 164.0291, 
+Predicted Market Sentiment: 0.11577205263157893</t>
         </is>
       </c>
     </row>

</xml_diff>